<commit_message>
cập nhật  mô hình
</commit_message>
<xml_diff>
--- a/tools/IP-Planning-Hardware-Requirements.xlsx
+++ b/tools/IP-Planning-Hardware-Requirements.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CEPH-Alone" sheetId="7" r:id="rId1"/>
-    <sheet name="OpenStack_Ceph-AIO" sheetId="8" r:id="rId2"/>
+    <sheet name="OpenStack_Ceph-AIO-Ubuntu" sheetId="8" r:id="rId2"/>
+    <sheet name="OpenStack_Ceph-AIO-CentOS" sheetId="9" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="42">
   <si>
     <t>Controller</t>
   </si>
@@ -148,6 +149,15 @@
   </si>
   <si>
     <t>IP PLANNING dành cho LAB OpenStack - CEPH-AIO</t>
+  </si>
+  <si>
+    <t>eno16777728</t>
+  </si>
+  <si>
+    <t>eno33554952</t>
+  </si>
+  <si>
+    <t>eno50332176</t>
   </si>
 </sst>
 </file>
@@ -412,7 +422,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -434,57 +444,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -529,6 +488,84 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -829,23 +866,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="20" t="s">
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="22"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="36"/>
     </row>
     <row r="3" spans="2:14" ht="33" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
@@ -889,7 +926,7 @@
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="26" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -903,30 +940,30 @@
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
-      <c r="H4" s="15">
-        <v>4</v>
-      </c>
-      <c r="I4" s="15">
+      <c r="H4" s="37">
+        <v>4</v>
+      </c>
+      <c r="I4" s="37">
         <v>2</v>
       </c>
-      <c r="J4" s="16">
+      <c r="J4" s="29">
         <v>40</v>
       </c>
-      <c r="K4" s="11">
+      <c r="K4" s="30">
         <v>60</v>
       </c>
-      <c r="L4" s="11">
+      <c r="L4" s="30">
         <v>60</v>
       </c>
-      <c r="M4" s="11">
+      <c r="M4" s="30">
         <v>60</v>
       </c>
-      <c r="N4" s="11">
+      <c r="N4" s="30">
         <v>60</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="13"/>
+      <c r="B5" s="27"/>
       <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
@@ -942,16 +979,16 @@
       <c r="G5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="30"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="13"/>
+      <c r="B6" s="27"/>
       <c r="C6" s="2" t="s">
         <v>23</v>
       </c>
@@ -963,16 +1000,16 @@
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="14"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="2" t="s">
         <v>26</v>
       </c>
@@ -980,16 +1017,16 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="30"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="26" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -1003,30 +1040,30 @@
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="15">
-        <v>4</v>
-      </c>
-      <c r="I8" s="15">
+      <c r="H8" s="37">
+        <v>4</v>
+      </c>
+      <c r="I8" s="37">
         <v>2</v>
       </c>
-      <c r="J8" s="16">
+      <c r="J8" s="29">
         <v>40</v>
       </c>
-      <c r="K8" s="11">
+      <c r="K8" s="30">
         <v>60</v>
       </c>
-      <c r="L8" s="11">
+      <c r="L8" s="30">
         <v>60</v>
       </c>
-      <c r="M8" s="11">
+      <c r="M8" s="30">
         <v>60</v>
       </c>
-      <c r="N8" s="11">
+      <c r="N8" s="30">
         <v>60</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="13"/>
+      <c r="B9" s="27"/>
       <c r="C9" s="2" t="s">
         <v>2</v>
       </c>
@@ -1042,16 +1079,16 @@
       <c r="G9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="11"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="30"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="13"/>
+      <c r="B10" s="27"/>
       <c r="C10" s="2" t="s">
         <v>23</v>
       </c>
@@ -1063,16 +1100,16 @@
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="14"/>
+      <c r="B11" s="28"/>
       <c r="C11" s="2" t="s">
         <v>26</v>
       </c>
@@ -1080,16 +1117,16 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="26" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1103,30 +1140,30 @@
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="15">
-        <v>4</v>
-      </c>
-      <c r="I12" s="15">
+      <c r="H12" s="37">
+        <v>4</v>
+      </c>
+      <c r="I12" s="37">
         <v>2</v>
       </c>
-      <c r="J12" s="16">
+      <c r="J12" s="29">
         <v>40</v>
       </c>
-      <c r="K12" s="11">
+      <c r="K12" s="30">
         <v>60</v>
       </c>
-      <c r="L12" s="11">
+      <c r="L12" s="30">
         <v>60</v>
       </c>
-      <c r="M12" s="11">
+      <c r="M12" s="30">
         <v>60</v>
       </c>
-      <c r="N12" s="11">
+      <c r="N12" s="30">
         <v>60</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="13"/>
+      <c r="B13" s="27"/>
       <c r="C13" s="2" t="s">
         <v>2</v>
       </c>
@@ -1142,16 +1179,16 @@
       <c r="G13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="13"/>
+      <c r="B14" s="27"/>
       <c r="C14" s="2" t="s">
         <v>23</v>
       </c>
@@ -1163,16 +1200,16 @@
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="11"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="14"/>
+      <c r="B15" s="28"/>
       <c r="C15" s="2" t="s">
         <v>26</v>
       </c>
@@ -1180,26 +1217,16 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="J4:J7"/>
-    <mergeCell ref="K4:K7"/>
-    <mergeCell ref="L4:L7"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:N2"/>
-    <mergeCell ref="M4:M7"/>
-    <mergeCell ref="N4:N7"/>
-    <mergeCell ref="I4:I7"/>
-    <mergeCell ref="H4:H7"/>
     <mergeCell ref="L12:L15"/>
     <mergeCell ref="M12:M15"/>
     <mergeCell ref="N12:N15"/>
@@ -1216,6 +1243,16 @@
     <mergeCell ref="L8:L11"/>
     <mergeCell ref="M8:M11"/>
     <mergeCell ref="N8:N11"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="J4:J7"/>
+    <mergeCell ref="K4:K7"/>
+    <mergeCell ref="L4:L7"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:N2"/>
+    <mergeCell ref="M4:M7"/>
+    <mergeCell ref="N4:N7"/>
+    <mergeCell ref="I4:I7"/>
+    <mergeCell ref="H4:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1225,8 +1262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1242,58 +1279,58 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="20" t="s">
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="22"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="36"/>
     </row>
     <row r="4" spans="2:14" ht="33" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="29" t="s">
+      <c r="F4" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="30" t="s">
+      <c r="G4" s="13" t="s">
         <v>25</v>
       </c>
       <c r="H4" s="10" t="s">
@@ -1319,254 +1356,273 @@
       </c>
     </row>
     <row r="5" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="D5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="33"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="27">
+      <c r="E5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="16"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="42">
         <v>6</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="37">
         <v>2</v>
       </c>
-      <c r="J5" s="16">
+      <c r="J5" s="29">
         <v>100</v>
       </c>
-      <c r="K5" s="11">
+      <c r="K5" s="30">
         <v>60</v>
       </c>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="30"/>
     </row>
     <row r="6" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="25"/>
-      <c r="C6" s="31" t="s">
+      <c r="B6" s="40"/>
+      <c r="C6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="35" t="s">
+      <c r="E6" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="36" t="s">
+      <c r="G6" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="27"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
     </row>
     <row r="7" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="37" t="s">
+      <c r="D7" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="37"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="27">
+      <c r="E7" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="20"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="42">
         <v>8</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="37">
+        <v>4</v>
+      </c>
+      <c r="J7" s="29">
+        <v>100</v>
+      </c>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="30"/>
+    </row>
+    <row r="8" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="40"/>
+      <c r="C8" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="J7" s="16">
-        <v>100</v>
-      </c>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
-    </row>
-    <row r="8" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="25"/>
-      <c r="C8" s="31" t="s">
+      <c r="D8" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="42"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="30"/>
+    </row>
+    <row r="9" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="42">
+        <v>8</v>
+      </c>
+      <c r="I9" s="37">
+        <v>4</v>
+      </c>
+      <c r="J9" s="29">
+        <v>60</v>
+      </c>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="30"/>
+    </row>
+    <row r="10" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="40"/>
+      <c r="C10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="35" t="s">
+      <c r="D10" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="36" t="s">
+      <c r="G10" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="27"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
-    </row>
-    <row r="9" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="32" t="s">
+      <c r="H10" s="42"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
+    </row>
+    <row r="11" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="37" t="s">
+      <c r="D11" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" s="37"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="27">
+      <c r="E11" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="20"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="42">
         <v>8</v>
       </c>
-      <c r="I9" s="15">
+      <c r="I11" s="37">
+        <v>4</v>
+      </c>
+      <c r="J11" s="29">
+        <v>60</v>
+      </c>
+      <c r="K11" s="30">
+        <v>50</v>
+      </c>
+      <c r="L11" s="30">
+        <v>50</v>
+      </c>
+      <c r="M11" s="30">
+        <v>50</v>
+      </c>
+      <c r="N11" s="30">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="40"/>
+      <c r="C12" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="J9" s="16">
-        <v>60</v>
-      </c>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="11"/>
-    </row>
-    <row r="10" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="25"/>
-      <c r="C10" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="35" t="s">
+      <c r="D12" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" s="35" t="s">
+      <c r="E12" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="36" t="s">
+      <c r="G12" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="27"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11"/>
-    </row>
-    <row r="11" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="37"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="27">
-        <v>4</v>
-      </c>
-      <c r="I11" s="15">
-        <v>2</v>
-      </c>
-      <c r="J11" s="16">
-        <v>60</v>
-      </c>
-      <c r="K11" s="11">
-        <v>50</v>
-      </c>
-      <c r="L11" s="11">
-        <v>50</v>
-      </c>
-      <c r="M11" s="11">
-        <v>50</v>
-      </c>
-      <c r="N11" s="11">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="25"/>
-      <c r="C12" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="39" t="s">
-        <v>4</v>
-      </c>
-      <c r="F12" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="H12" s="27"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
     </row>
     <row r="13" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="26"/>
-      <c r="C13" s="31" t="s">
+      <c r="B13" s="41"/>
+      <c r="C13" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="41" t="s">
+      <c r="D13" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="F13" s="41"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
+      <c r="E13" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="24"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="H3:N3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
     <mergeCell ref="M11:M13"/>
     <mergeCell ref="N11:N13"/>
     <mergeCell ref="B2:N2"/>
@@ -1583,15 +1639,385 @@
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
     <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:N13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="19" style="48" customWidth="1"/>
+    <col min="4" max="4" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="14" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:14" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="51"/>
+    </row>
+    <row r="3" spans="2:14" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="36"/>
+    </row>
+    <row r="4" spans="2:14" ht="33" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="16"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="42">
+        <v>6</v>
+      </c>
+      <c r="I5" s="37">
+        <v>2</v>
+      </c>
+      <c r="J5" s="29">
+        <v>100</v>
+      </c>
+      <c r="K5" s="30">
+        <v>60</v>
+      </c>
+      <c r="L5" s="30"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="30"/>
+    </row>
+    <row r="6" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="40"/>
+      <c r="C6" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="42"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
+    </row>
+    <row r="7" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="20"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="42">
+        <v>8</v>
+      </c>
+      <c r="I7" s="37">
+        <v>4</v>
+      </c>
+      <c r="J7" s="29">
+        <v>100</v>
+      </c>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="30"/>
+    </row>
+    <row r="8" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="40"/>
+      <c r="C8" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="42"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="30"/>
+    </row>
+    <row r="9" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="42">
+        <v>8</v>
+      </c>
+      <c r="I9" s="37">
+        <v>4</v>
+      </c>
+      <c r="J9" s="29">
+        <v>60</v>
+      </c>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="30"/>
+    </row>
+    <row r="10" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="40"/>
+      <c r="C10" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="42"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
+    </row>
+    <row r="11" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="20"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="42">
+        <v>8</v>
+      </c>
+      <c r="I11" s="37">
+        <v>4</v>
+      </c>
+      <c r="J11" s="29">
+        <v>60</v>
+      </c>
+      <c r="K11" s="30">
+        <v>50</v>
+      </c>
+      <c r="L11" s="30">
+        <v>50</v>
+      </c>
+      <c r="M11" s="30">
+        <v>50</v>
+      </c>
+      <c r="N11" s="30">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="40"/>
+      <c r="C12" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" s="42"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
+    </row>
+    <row r="13" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="41"/>
+      <c r="C13" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="24"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
+    </row>
+  </sheetData>
+  <mergeCells count="35">
     <mergeCell ref="M9:M10"/>
     <mergeCell ref="N9:N10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="I11:I13"/>
+    <mergeCell ref="J11:J13"/>
+    <mergeCell ref="K11:K13"/>
+    <mergeCell ref="L11:L13"/>
+    <mergeCell ref="M11:M13"/>
+    <mergeCell ref="N11:N13"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="N5:N6"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="K7:K8"/>
     <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="B2:N2"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="H3:N3"/>
     <mergeCell ref="B5:B6"/>
@@ -1601,7 +2027,6 @@
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
Cập nhật hướng dẫn
Cập nhật hướng dẫn
</commit_message>
<xml_diff>
--- a/tools/IP-Planning-Hardware-Requirements.xlsx
+++ b/tools/IP-Planning-Hardware-Requirements.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CEPH-Alone" sheetId="7" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="52">
   <si>
     <t>Controller</t>
   </si>
@@ -167,6 +167,29 @@
   </si>
   <si>
     <t>10.10.30.71</t>
+  </si>
+  <si>
+    <t>10.10.10.81</t>
+  </si>
+  <si>
+    <t>172.16.69.81</t>
+  </si>
+  <si>
+    <t>CentOS7
+Client1</t>
+  </si>
+  <si>
+    <t>Ubuntu14.04
+Client2</t>
+  </si>
+  <si>
+    <t>10.10.10.82</t>
+  </si>
+  <si>
+    <t>172.16.69.82</t>
+  </si>
+  <si>
+    <t>IP PLANNING dành cho LAB - CEPH-AIO</t>
   </si>
 </sst>
 </file>
@@ -422,7 +445,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -507,61 +530,73 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -863,23 +898,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="41" t="s">
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="42"/>
-      <c r="M2" s="42"/>
-      <c r="N2" s="43"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="42"/>
     </row>
     <row r="3" spans="2:14" ht="33" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
@@ -923,7 +958,7 @@
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="32" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -937,30 +972,30 @@
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
-      <c r="H4" s="36">
-        <v>4</v>
-      </c>
-      <c r="I4" s="36">
+      <c r="H4" s="43">
+        <v>4</v>
+      </c>
+      <c r="I4" s="43">
         <v>2</v>
       </c>
-      <c r="J4" s="37">
+      <c r="J4" s="35">
         <v>40</v>
       </c>
-      <c r="K4" s="32">
+      <c r="K4" s="36">
         <v>60</v>
       </c>
-      <c r="L4" s="32">
+      <c r="L4" s="36">
         <v>60</v>
       </c>
-      <c r="M4" s="32">
+      <c r="M4" s="36">
         <v>60</v>
       </c>
-      <c r="N4" s="32">
+      <c r="N4" s="36">
         <v>60</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="34"/>
+      <c r="B5" s="33"/>
       <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
@@ -976,16 +1011,16 @@
       <c r="G5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="37"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="32"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="36"/>
+      <c r="M5" s="36"/>
+      <c r="N5" s="36"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="34"/>
+      <c r="B6" s="33"/>
       <c r="C6" s="2" t="s">
         <v>23</v>
       </c>
@@ -997,16 +1032,16 @@
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="32"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="36"/>
+      <c r="N6" s="36"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="35"/>
+      <c r="B7" s="34"/>
       <c r="C7" s="2" t="s">
         <v>26</v>
       </c>
@@ -1014,16 +1049,16 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="32"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
+      <c r="M7" s="36"/>
+      <c r="N7" s="36"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="32" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -1037,30 +1072,30 @@
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="36">
-        <v>4</v>
-      </c>
-      <c r="I8" s="36">
+      <c r="H8" s="43">
+        <v>4</v>
+      </c>
+      <c r="I8" s="43">
         <v>2</v>
       </c>
-      <c r="J8" s="37">
+      <c r="J8" s="35">
         <v>40</v>
       </c>
-      <c r="K8" s="32">
+      <c r="K8" s="36">
         <v>60</v>
       </c>
-      <c r="L8" s="32">
+      <c r="L8" s="36">
         <v>60</v>
       </c>
-      <c r="M8" s="32">
+      <c r="M8" s="36">
         <v>60</v>
       </c>
-      <c r="N8" s="32">
+      <c r="N8" s="36">
         <v>60</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="34"/>
+      <c r="B9" s="33"/>
       <c r="C9" s="2" t="s">
         <v>2</v>
       </c>
@@ -1076,16 +1111,16 @@
       <c r="G9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="32"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="36"/>
+      <c r="M9" s="36"/>
+      <c r="N9" s="36"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="34"/>
+      <c r="B10" s="33"/>
       <c r="C10" s="2" t="s">
         <v>23</v>
       </c>
@@ -1097,16 +1132,16 @@
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="37"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="32"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="36"/>
+      <c r="M10" s="36"/>
+      <c r="N10" s="36"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="35"/>
+      <c r="B11" s="34"/>
       <c r="C11" s="2" t="s">
         <v>26</v>
       </c>
@@ -1114,16 +1149,16 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="37"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="32"/>
-      <c r="N11" s="32"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="36"/>
+      <c r="N11" s="36"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="32" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1137,30 +1172,30 @@
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="36">
-        <v>4</v>
-      </c>
-      <c r="I12" s="36">
+      <c r="H12" s="43">
+        <v>4</v>
+      </c>
+      <c r="I12" s="43">
         <v>2</v>
       </c>
-      <c r="J12" s="37">
+      <c r="J12" s="35">
         <v>40</v>
       </c>
-      <c r="K12" s="32">
+      <c r="K12" s="36">
         <v>60</v>
       </c>
-      <c r="L12" s="32">
+      <c r="L12" s="36">
         <v>60</v>
       </c>
-      <c r="M12" s="32">
+      <c r="M12" s="36">
         <v>60</v>
       </c>
-      <c r="N12" s="32">
+      <c r="N12" s="36">
         <v>60</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="34"/>
+      <c r="B13" s="33"/>
       <c r="C13" s="2" t="s">
         <v>2</v>
       </c>
@@ -1176,16 +1211,16 @@
       <c r="G13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="36"/>
-      <c r="I13" s="36"/>
-      <c r="J13" s="37"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="32"/>
-      <c r="N13" s="32"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="36"/>
+      <c r="N13" s="36"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="34"/>
+      <c r="B14" s="33"/>
       <c r="C14" s="2" t="s">
         <v>23</v>
       </c>
@@ -1197,16 +1232,16 @@
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="32"/>
-      <c r="L14" s="32"/>
-      <c r="M14" s="32"/>
-      <c r="N14" s="32"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="36"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="36"/>
+      <c r="N14" s="36"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="35"/>
+      <c r="B15" s="34"/>
       <c r="C15" s="2" t="s">
         <v>26</v>
       </c>
@@ -1214,26 +1249,16 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="32"/>
-      <c r="M15" s="32"/>
-      <c r="N15" s="32"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="36"/>
+      <c r="M15" s="36"/>
+      <c r="N15" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="J4:J7"/>
-    <mergeCell ref="K4:K7"/>
-    <mergeCell ref="L4:L7"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:N2"/>
-    <mergeCell ref="M4:M7"/>
-    <mergeCell ref="N4:N7"/>
-    <mergeCell ref="I4:I7"/>
-    <mergeCell ref="H4:H7"/>
     <mergeCell ref="L12:L15"/>
     <mergeCell ref="M12:M15"/>
     <mergeCell ref="N12:N15"/>
@@ -1250,6 +1275,16 @@
     <mergeCell ref="L8:L11"/>
     <mergeCell ref="M8:M11"/>
     <mergeCell ref="N8:N11"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="J4:J7"/>
+    <mergeCell ref="K4:K7"/>
+    <mergeCell ref="L4:L7"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:N2"/>
+    <mergeCell ref="M4:M7"/>
+    <mergeCell ref="N4:N7"/>
+    <mergeCell ref="I4:I7"/>
+    <mergeCell ref="H4:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1257,59 +1292,63 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:N13"/>
+  <dimension ref="B2:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="A4" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="15.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="9" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.140625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="14" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="19.85546875" style="53" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="53" customWidth="1"/>
+    <col min="4" max="4" width="16" style="53" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="53" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="53" customWidth="1"/>
+    <col min="7" max="7" width="9" style="53" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" style="53" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" style="53" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="9.5703125" style="53" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="9.42578125" style="53" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="50"/>
-    </row>
-    <row r="3" spans="2:14" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="38" t="s">
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="46"/>
+    </row>
+    <row r="3" spans="2:14" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="41" t="s">
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="43"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="42"/>
     </row>
     <row r="4" spans="2:14" ht="33" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
@@ -1353,7 +1392,7 @@
       </c>
     </row>
     <row r="5" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="47" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="11" t="s">
@@ -1367,24 +1406,24 @@
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="17"/>
-      <c r="H5" s="46">
+      <c r="H5" s="50">
         <v>6</v>
       </c>
-      <c r="I5" s="36">
+      <c r="I5" s="43">
         <v>2</v>
       </c>
-      <c r="J5" s="37">
+      <c r="J5" s="35">
         <v>100</v>
       </c>
-      <c r="K5" s="32">
+      <c r="K5" s="36">
         <v>60</v>
       </c>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="32"/>
+      <c r="L5" s="36"/>
+      <c r="M5" s="36"/>
+      <c r="N5" s="36"/>
     </row>
     <row r="6" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="45"/>
+      <c r="B6" s="48"/>
       <c r="C6" s="14" t="s">
         <v>2</v>
       </c>
@@ -1400,16 +1439,16 @@
       <c r="G6" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="46"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="32"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="36"/>
+      <c r="N6" s="36"/>
     </row>
     <row r="7" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="47" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="15" t="s">
@@ -1423,22 +1462,22 @@
       </c>
       <c r="F7" s="20"/>
       <c r="G7" s="21"/>
-      <c r="H7" s="46">
+      <c r="H7" s="50">
         <v>8</v>
       </c>
-      <c r="I7" s="36">
-        <v>4</v>
-      </c>
-      <c r="J7" s="37">
+      <c r="I7" s="43">
+        <v>4</v>
+      </c>
+      <c r="J7" s="35">
         <v>100</v>
       </c>
-      <c r="K7" s="32"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="32"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
+      <c r="M7" s="36"/>
+      <c r="N7" s="36"/>
     </row>
     <row r="8" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="45"/>
+      <c r="B8" s="48"/>
       <c r="C8" s="14" t="s">
         <v>2</v>
       </c>
@@ -1454,16 +1493,16 @@
       <c r="G8" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="46"/>
-      <c r="I8" s="36"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="32"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="36"/>
+      <c r="N8" s="36"/>
     </row>
     <row r="9" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="47" t="s">
         <v>36</v>
       </c>
       <c r="C9" s="15" t="s">
@@ -1477,22 +1516,22 @@
       </c>
       <c r="F9" s="20"/>
       <c r="G9" s="21"/>
-      <c r="H9" s="46">
+      <c r="H9" s="50">
         <v>8</v>
       </c>
-      <c r="I9" s="36">
-        <v>4</v>
-      </c>
-      <c r="J9" s="37">
+      <c r="I9" s="43">
+        <v>4</v>
+      </c>
+      <c r="J9" s="35">
         <v>60</v>
       </c>
-      <c r="K9" s="32"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="32"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="36"/>
+      <c r="M9" s="36"/>
+      <c r="N9" s="36"/>
     </row>
     <row r="10" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="45"/>
+      <c r="B10" s="48"/>
       <c r="C10" s="14" t="s">
         <v>2</v>
       </c>
@@ -1508,16 +1547,16 @@
       <c r="G10" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="46"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="37"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="32"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="36"/>
+      <c r="M10" s="36"/>
+      <c r="N10" s="36"/>
     </row>
     <row r="11" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="47" t="s">
         <v>37</v>
       </c>
       <c r="C11" s="15" t="s">
@@ -1531,30 +1570,30 @@
       </c>
       <c r="F11" s="20"/>
       <c r="G11" s="21"/>
-      <c r="H11" s="46">
+      <c r="H11" s="50">
         <v>8</v>
       </c>
-      <c r="I11" s="36">
-        <v>4</v>
-      </c>
-      <c r="J11" s="37">
+      <c r="I11" s="43">
+        <v>4</v>
+      </c>
+      <c r="J11" s="35">
         <v>60</v>
       </c>
-      <c r="K11" s="32">
+      <c r="K11" s="36">
         <v>50</v>
       </c>
-      <c r="L11" s="32">
+      <c r="L11" s="36">
         <v>50</v>
       </c>
-      <c r="M11" s="32">
+      <c r="M11" s="36">
         <v>50</v>
       </c>
-      <c r="N11" s="32">
+      <c r="N11" s="36">
         <v>50</v>
       </c>
     </row>
     <row r="12" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="45"/>
+      <c r="B12" s="48"/>
       <c r="C12" s="15" t="s">
         <v>2</v>
       </c>
@@ -1570,16 +1609,16 @@
       <c r="G12" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="46"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="32"/>
-      <c r="L12" s="32"/>
-      <c r="M12" s="32"/>
-      <c r="N12" s="32"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="36"/>
+      <c r="N12" s="36"/>
     </row>
     <row r="13" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="47"/>
+      <c r="B13" s="49"/>
       <c r="C13" s="14" t="s">
         <v>23</v>
       </c>
@@ -1591,16 +1630,159 @@
       </c>
       <c r="F13" s="24"/>
       <c r="G13" s="25"/>
-      <c r="H13" s="46"/>
-      <c r="I13" s="36"/>
-      <c r="J13" s="37"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="32"/>
-      <c r="N13" s="32"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="36"/>
+      <c r="N13" s="36"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="51" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="20"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="50">
+        <v>2</v>
+      </c>
+      <c r="I14" s="43">
+        <v>2</v>
+      </c>
+      <c r="J14" s="35">
+        <v>60</v>
+      </c>
+      <c r="K14" s="36"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="36"/>
+      <c r="N14" s="36"/>
+    </row>
+    <row r="15" spans="2:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="48"/>
+      <c r="C15" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" s="50"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="36"/>
+      <c r="M15" s="36"/>
+      <c r="N15" s="36"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B16" s="52" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="20"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="50">
+        <v>2</v>
+      </c>
+      <c r="I16" s="43">
+        <v>2</v>
+      </c>
+      <c r="J16" s="35">
+        <v>60</v>
+      </c>
+      <c r="K16" s="36"/>
+      <c r="L16" s="36"/>
+      <c r="M16" s="36"/>
+      <c r="N16" s="36"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17" s="34"/>
+      <c r="C17" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="H17" s="50"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="36"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="36"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
+  <mergeCells count="51">
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="H3:N3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
     <mergeCell ref="M11:M13"/>
     <mergeCell ref="N11:N13"/>
     <mergeCell ref="B2:N2"/>
@@ -1617,7 +1799,500 @@
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
     <mergeCell ref="K9:K10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:N17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" style="31" customWidth="1"/>
+    <col min="4" max="4" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="14" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:14" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="44" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="46"/>
+    </row>
+    <row r="3" spans="2:14" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="42"/>
+    </row>
+    <row r="4" spans="2:14" ht="33" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="54" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="16"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="50">
+        <v>6</v>
+      </c>
+      <c r="I5" s="43">
+        <v>2</v>
+      </c>
+      <c r="J5" s="35">
+        <v>100</v>
+      </c>
+      <c r="K5" s="36">
+        <v>60</v>
+      </c>
+      <c r="L5" s="36"/>
+      <c r="M5" s="36"/>
+      <c r="N5" s="36"/>
+    </row>
+    <row r="6" spans="2:14" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="48"/>
+      <c r="C6" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="50"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="36"/>
+      <c r="N6" s="36"/>
+    </row>
+    <row r="7" spans="2:14" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="20"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="50">
+        <v>8</v>
+      </c>
+      <c r="I7" s="43">
+        <v>4</v>
+      </c>
+      <c r="J7" s="35">
+        <v>100</v>
+      </c>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
+      <c r="M7" s="36"/>
+      <c r="N7" s="36"/>
+    </row>
+    <row r="8" spans="2:14" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="48"/>
+      <c r="C8" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="50"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="36"/>
+      <c r="N8" s="36"/>
+    </row>
+    <row r="9" spans="2:14" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="47" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="50">
+        <v>8</v>
+      </c>
+      <c r="I9" s="43">
+        <v>4</v>
+      </c>
+      <c r="J9" s="35">
+        <v>60</v>
+      </c>
+      <c r="K9" s="36"/>
+      <c r="L9" s="36"/>
+      <c r="M9" s="36"/>
+      <c r="N9" s="36"/>
+    </row>
+    <row r="10" spans="2:14" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="48"/>
+      <c r="C10" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="50"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="36"/>
+      <c r="M10" s="36"/>
+      <c r="N10" s="36"/>
+    </row>
+    <row r="11" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="47" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="20"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="50">
+        <v>8</v>
+      </c>
+      <c r="I11" s="43">
+        <v>4</v>
+      </c>
+      <c r="J11" s="35">
+        <v>60</v>
+      </c>
+      <c r="K11" s="36">
+        <v>50</v>
+      </c>
+      <c r="L11" s="36">
+        <v>50</v>
+      </c>
+      <c r="M11" s="36">
+        <v>50</v>
+      </c>
+      <c r="N11" s="36">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="48"/>
+      <c r="C12" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" s="50"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="36"/>
+      <c r="N12" s="36"/>
+    </row>
+    <row r="13" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="49"/>
+      <c r="C13" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="24"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="36"/>
+      <c r="N13" s="36"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="51" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="20"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="50">
+        <v>2</v>
+      </c>
+      <c r="I14" s="43">
+        <v>2</v>
+      </c>
+      <c r="J14" s="35">
+        <v>60</v>
+      </c>
+      <c r="K14" s="36"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="36"/>
+      <c r="N14" s="36"/>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B15" s="48"/>
+      <c r="C15" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" s="50"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="36"/>
+      <c r="M15" s="36"/>
+      <c r="N15" s="36"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B16" s="52" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="20"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="50">
+        <v>2</v>
+      </c>
+      <c r="I16" s="43">
+        <v>2</v>
+      </c>
+      <c r="J16" s="35">
+        <v>60</v>
+      </c>
+      <c r="K16" s="36"/>
+      <c r="L16" s="36"/>
+      <c r="M16" s="36"/>
+      <c r="N16" s="36"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17" s="34"/>
+      <c r="C17" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="H17" s="50"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="36"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="36"/>
+    </row>
+  </sheetData>
+  <mergeCells count="51">
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="L11:L13"/>
+    <mergeCell ref="M11:M13"/>
+    <mergeCell ref="N11:N13"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
     <mergeCell ref="L9:L10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="I11:I13"/>
+    <mergeCell ref="J11:J13"/>
+    <mergeCell ref="K11:K13"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="N7:N8"/>
     <mergeCell ref="M9:M10"/>
     <mergeCell ref="N9:N10"/>
     <mergeCell ref="B7:B8"/>
@@ -1625,7 +2300,7 @@
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="B2:N2"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="H3:N3"/>
     <mergeCell ref="B5:B6"/>
@@ -1640,392 +2315,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:N13"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="15.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="19" style="31" customWidth="1"/>
-    <col min="4" max="4" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="9" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.140625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="14" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:14" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="50"/>
-    </row>
-    <row r="3" spans="2:14" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="43"/>
-    </row>
-    <row r="4" spans="2:14" ht="33" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="L4" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="N4" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="16"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="46">
-        <v>6</v>
-      </c>
-      <c r="I5" s="36">
-        <v>2</v>
-      </c>
-      <c r="J5" s="37">
-        <v>100</v>
-      </c>
-      <c r="K5" s="32">
-        <v>60</v>
-      </c>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="32"/>
-    </row>
-    <row r="6" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="45"/>
-      <c r="C6" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" s="46"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="32"/>
-    </row>
-    <row r="7" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="44" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="46">
-        <v>8</v>
-      </c>
-      <c r="I7" s="36">
-        <v>4</v>
-      </c>
-      <c r="J7" s="37">
-        <v>100</v>
-      </c>
-      <c r="K7" s="32"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="32"/>
-    </row>
-    <row r="8" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="45"/>
-      <c r="C8" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" s="46"/>
-      <c r="I8" s="36"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="32"/>
-    </row>
-    <row r="9" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="46">
-        <v>8</v>
-      </c>
-      <c r="I9" s="36">
-        <v>4</v>
-      </c>
-      <c r="J9" s="37">
-        <v>60</v>
-      </c>
-      <c r="K9" s="32"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="32"/>
-    </row>
-    <row r="10" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="45"/>
-      <c r="C10" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" s="46"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="37"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="32"/>
-    </row>
-    <row r="11" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="44" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="46">
-        <v>8</v>
-      </c>
-      <c r="I11" s="36">
-        <v>4</v>
-      </c>
-      <c r="J11" s="37">
-        <v>60</v>
-      </c>
-      <c r="K11" s="32">
-        <v>50</v>
-      </c>
-      <c r="L11" s="32">
-        <v>50</v>
-      </c>
-      <c r="M11" s="32">
-        <v>50</v>
-      </c>
-      <c r="N11" s="32">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="45"/>
-      <c r="C12" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="F12" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="H12" s="46"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="32"/>
-      <c r="L12" s="32"/>
-      <c r="M12" s="32"/>
-      <c r="N12" s="32"/>
-    </row>
-    <row r="13" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="47"/>
-      <c r="C13" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="F13" s="24"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="46"/>
-      <c r="I13" s="36"/>
-      <c r="J13" s="37"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="32"/>
-      <c r="N13" s="32"/>
-    </row>
-  </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="H3:N3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="H11:H13"/>
-    <mergeCell ref="I11:I13"/>
-    <mergeCell ref="J11:J13"/>
-    <mergeCell ref="K11:K13"/>
-    <mergeCell ref="L11:L13"/>
-    <mergeCell ref="M11:M13"/>
-    <mergeCell ref="N11:N13"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
fix content install luminous Ubuntu & Cent
</commit_message>
<xml_diff>
--- a/tools/IP-Planning-Hardware-Requirements.xlsx
+++ b/tools/IP-Planning-Hardware-Requirements.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="54">
   <si>
     <t>Controller</t>
   </si>
@@ -186,10 +186,16 @@
     <t>172.16.69.150</t>
   </si>
   <si>
-    <t>10.10.20.72</t>
-  </si>
-  <si>
-    <t>10.10.10.72</t>
+    <t>10.10.20.75</t>
+  </si>
+  <si>
+    <t>10.10.10.75</t>
+  </si>
+  <si>
+    <t>10.10.20.76</t>
+  </si>
+  <si>
+    <t>10.10.10.76</t>
   </si>
 </sst>
 </file>
@@ -548,40 +554,49 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -590,19 +605,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -909,23 +915,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="47" t="s">
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="49"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="43"/>
     </row>
     <row r="3" spans="2:14" ht="33" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
@@ -969,7 +975,7 @@
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="44" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="35" t="s">
@@ -987,30 +993,30 @@
       <c r="G4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="42">
-        <v>4</v>
-      </c>
-      <c r="I4" s="42">
+      <c r="H4" s="46">
+        <v>4</v>
+      </c>
+      <c r="I4" s="46">
         <v>2</v>
       </c>
-      <c r="J4" s="43">
+      <c r="J4" s="47">
         <v>40</v>
       </c>
-      <c r="K4" s="38">
+      <c r="K4" s="48">
         <v>40</v>
       </c>
-      <c r="L4" s="38">
-        <v>60</v>
-      </c>
-      <c r="M4" s="38">
-        <v>60</v>
-      </c>
-      <c r="N4" s="38">
+      <c r="L4" s="48">
+        <v>60</v>
+      </c>
+      <c r="M4" s="48">
+        <v>60</v>
+      </c>
+      <c r="N4" s="48">
         <v>60</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="40"/>
+      <c r="B5" s="45"/>
       <c r="C5" s="35" t="s">
         <v>2</v>
       </c>
@@ -1022,16 +1028,16 @@
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
-      <c r="M5" s="38"/>
-      <c r="N5" s="38"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="48"/>
+      <c r="M5" s="48"/>
+      <c r="N5" s="48"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="40"/>
+      <c r="B6" s="45"/>
       <c r="C6" s="35" t="s">
         <v>23</v>
       </c>
@@ -1043,16 +1049,16 @@
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="38"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="38"/>
-      <c r="N6" s="38"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="48"/>
+      <c r="N6" s="48"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="44" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="35" t="s">
@@ -1070,30 +1076,30 @@
       <c r="G7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="42">
-        <v>4</v>
-      </c>
-      <c r="I7" s="42">
+      <c r="H7" s="46">
+        <v>4</v>
+      </c>
+      <c r="I7" s="46">
         <v>2</v>
       </c>
-      <c r="J7" s="43">
+      <c r="J7" s="47">
         <v>40</v>
       </c>
-      <c r="K7" s="38">
+      <c r="K7" s="48">
         <v>40</v>
       </c>
-      <c r="L7" s="38">
-        <v>60</v>
-      </c>
-      <c r="M7" s="38">
-        <v>60</v>
-      </c>
-      <c r="N7" s="38">
+      <c r="L7" s="48">
+        <v>60</v>
+      </c>
+      <c r="M7" s="48">
+        <v>60</v>
+      </c>
+      <c r="N7" s="48">
         <v>60</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="40"/>
+      <c r="B8" s="45"/>
       <c r="C8" s="35" t="s">
         <v>2</v>
       </c>
@@ -1105,16 +1111,16 @@
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="38"/>
-      <c r="L8" s="38"/>
-      <c r="M8" s="38"/>
-      <c r="N8" s="38"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="48"/>
+      <c r="L8" s="48"/>
+      <c r="M8" s="48"/>
+      <c r="N8" s="48"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="41"/>
+      <c r="B9" s="49"/>
       <c r="C9" s="35" t="s">
         <v>23</v>
       </c>
@@ -1126,13 +1132,13 @@
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="38"/>
-      <c r="L9" s="38"/>
-      <c r="M9" s="38"/>
-      <c r="N9" s="38"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="48"/>
+      <c r="L9" s="48"/>
+      <c r="M9" s="48"/>
+      <c r="N9" s="48"/>
     </row>
     <row r="10" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="37" t="s">
@@ -1177,6 +1183,14 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="M7:M9"/>
+    <mergeCell ref="N7:N9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="J7:J9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="L7:L9"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="H2:N2"/>
     <mergeCell ref="B4:B6"/>
@@ -1187,14 +1201,6 @@
     <mergeCell ref="L4:L6"/>
     <mergeCell ref="M4:M6"/>
     <mergeCell ref="N4:N6"/>
-    <mergeCell ref="M7:M9"/>
-    <mergeCell ref="N7:N9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="J7:J9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="L7:L9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="77" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -1209,7 +1215,7 @@
   <dimension ref="B2:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1227,23 +1233,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="47" t="s">
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="49"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="43"/>
     </row>
     <row r="3" spans="2:14" ht="33" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
@@ -1287,7 +1293,7 @@
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="44" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="32" t="s">
@@ -1305,72 +1311,72 @@
       <c r="G4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="42">
-        <v>4</v>
-      </c>
-      <c r="I4" s="42">
+      <c r="H4" s="46">
+        <v>4</v>
+      </c>
+      <c r="I4" s="46">
         <v>2</v>
       </c>
-      <c r="J4" s="43">
+      <c r="J4" s="47">
         <v>40</v>
       </c>
-      <c r="K4" s="38">
+      <c r="K4" s="48">
         <v>40</v>
       </c>
-      <c r="L4" s="38">
-        <v>60</v>
-      </c>
-      <c r="M4" s="38">
-        <v>60</v>
-      </c>
-      <c r="N4" s="38">
+      <c r="L4" s="48">
+        <v>60</v>
+      </c>
+      <c r="M4" s="48">
+        <v>60</v>
+      </c>
+      <c r="N4" s="48">
         <v>60</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="40"/>
+      <c r="B5" s="45"/>
       <c r="C5" s="32" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
-      <c r="M5" s="38"/>
-      <c r="N5" s="38"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="48"/>
+      <c r="M5" s="48"/>
+      <c r="N5" s="48"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="40"/>
+      <c r="B6" s="45"/>
       <c r="C6" s="32" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>4</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="38"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="38"/>
-      <c r="N6" s="38"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="48"/>
+      <c r="N6" s="48"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="44" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="32" t="s">
@@ -1388,72 +1394,80 @@
       <c r="G7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="42">
-        <v>4</v>
-      </c>
-      <c r="I7" s="42">
+      <c r="H7" s="46">
+        <v>4</v>
+      </c>
+      <c r="I7" s="46">
         <v>2</v>
       </c>
-      <c r="J7" s="43">
+      <c r="J7" s="47">
         <v>40</v>
       </c>
-      <c r="K7" s="38">
+      <c r="K7" s="48">
         <v>40</v>
       </c>
-      <c r="L7" s="38">
-        <v>60</v>
-      </c>
-      <c r="M7" s="38">
-        <v>60</v>
-      </c>
-      <c r="N7" s="38">
+      <c r="L7" s="48">
+        <v>60</v>
+      </c>
+      <c r="M7" s="48">
+        <v>60</v>
+      </c>
+      <c r="N7" s="48">
         <v>60</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="40"/>
+      <c r="B8" s="45"/>
       <c r="C8" s="32" t="s">
         <v>2</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="38"/>
-      <c r="L8" s="38"/>
-      <c r="M8" s="38"/>
-      <c r="N8" s="38"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="48"/>
+      <c r="L8" s="48"/>
+      <c r="M8" s="48"/>
+      <c r="N8" s="48"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="41"/>
+      <c r="B9" s="49"/>
       <c r="C9" s="32" t="s">
         <v>23</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>4</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="38"/>
-      <c r="L9" s="38"/>
-      <c r="M9" s="38"/>
-      <c r="N9" s="38"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="48"/>
+      <c r="L9" s="48"/>
+      <c r="M9" s="48"/>
+      <c r="N9" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="M7:M9"/>
+    <mergeCell ref="N7:N9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="J7:J9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="L7:L9"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="H2:N2"/>
     <mergeCell ref="B4:B6"/>
@@ -1464,14 +1478,6 @@
     <mergeCell ref="L4:L6"/>
     <mergeCell ref="M4:M6"/>
     <mergeCell ref="N4:N6"/>
-    <mergeCell ref="M7:M9"/>
-    <mergeCell ref="N7:N9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="J7:J9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="L7:L9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="78" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -1499,23 +1505,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="47" t="s">
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="49"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="43"/>
     </row>
     <row r="3" spans="2:14" ht="33" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
@@ -1559,7 +1565,7 @@
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="44" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1573,30 +1579,30 @@
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
-      <c r="H4" s="42">
-        <v>4</v>
-      </c>
-      <c r="I4" s="42">
+      <c r="H4" s="46">
+        <v>4</v>
+      </c>
+      <c r="I4" s="46">
         <v>2</v>
       </c>
-      <c r="J4" s="43">
+      <c r="J4" s="47">
         <v>40</v>
       </c>
-      <c r="K4" s="38">
-        <v>60</v>
-      </c>
-      <c r="L4" s="38">
-        <v>60</v>
-      </c>
-      <c r="M4" s="38">
-        <v>60</v>
-      </c>
-      <c r="N4" s="38">
+      <c r="K4" s="48">
+        <v>60</v>
+      </c>
+      <c r="L4" s="48">
+        <v>60</v>
+      </c>
+      <c r="M4" s="48">
+        <v>60</v>
+      </c>
+      <c r="N4" s="48">
         <v>60</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="40"/>
+      <c r="B5" s="45"/>
       <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
@@ -1612,16 +1618,16 @@
       <c r="G5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
-      <c r="M5" s="38"/>
-      <c r="N5" s="38"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="48"/>
+      <c r="M5" s="48"/>
+      <c r="N5" s="48"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="40"/>
+      <c r="B6" s="45"/>
       <c r="C6" s="2" t="s">
         <v>23</v>
       </c>
@@ -1633,16 +1639,16 @@
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="38"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="38"/>
-      <c r="N6" s="38"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="48"/>
+      <c r="N6" s="48"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="41"/>
+      <c r="B7" s="49"/>
       <c r="C7" s="2" t="s">
         <v>26</v>
       </c>
@@ -1650,16 +1656,16 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="38"/>
-      <c r="N7" s="38"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="48"/>
+      <c r="M7" s="48"/>
+      <c r="N7" s="48"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="44" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -1673,30 +1679,30 @@
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="42">
-        <v>4</v>
-      </c>
-      <c r="I8" s="42">
+      <c r="H8" s="46">
+        <v>4</v>
+      </c>
+      <c r="I8" s="46">
         <v>2</v>
       </c>
-      <c r="J8" s="43">
+      <c r="J8" s="47">
         <v>40</v>
       </c>
-      <c r="K8" s="38">
-        <v>60</v>
-      </c>
-      <c r="L8" s="38">
-        <v>60</v>
-      </c>
-      <c r="M8" s="38">
-        <v>60</v>
-      </c>
-      <c r="N8" s="38">
+      <c r="K8" s="48">
+        <v>60</v>
+      </c>
+      <c r="L8" s="48">
+        <v>60</v>
+      </c>
+      <c r="M8" s="48">
+        <v>60</v>
+      </c>
+      <c r="N8" s="48">
         <v>60</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="40"/>
+      <c r="B9" s="45"/>
       <c r="C9" s="2" t="s">
         <v>2</v>
       </c>
@@ -1712,16 +1718,16 @@
       <c r="G9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="38"/>
-      <c r="L9" s="38"/>
-      <c r="M9" s="38"/>
-      <c r="N9" s="38"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="48"/>
+      <c r="L9" s="48"/>
+      <c r="M9" s="48"/>
+      <c r="N9" s="48"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="40"/>
+      <c r="B10" s="45"/>
       <c r="C10" s="2" t="s">
         <v>23</v>
       </c>
@@ -1733,16 +1739,16 @@
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="38"/>
-      <c r="N10" s="38"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="48"/>
+      <c r="M10" s="48"/>
+      <c r="N10" s="48"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="41"/>
+      <c r="B11" s="49"/>
       <c r="C11" s="2" t="s">
         <v>26</v>
       </c>
@@ -1750,16 +1756,16 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="38"/>
-      <c r="L11" s="38"/>
-      <c r="M11" s="38"/>
-      <c r="N11" s="38"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="47"/>
+      <c r="K11" s="48"/>
+      <c r="L11" s="48"/>
+      <c r="M11" s="48"/>
+      <c r="N11" s="48"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="44" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1773,30 +1779,30 @@
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="42">
-        <v>4</v>
-      </c>
-      <c r="I12" s="42">
+      <c r="H12" s="46">
+        <v>4</v>
+      </c>
+      <c r="I12" s="46">
         <v>2</v>
       </c>
-      <c r="J12" s="43">
+      <c r="J12" s="47">
         <v>40</v>
       </c>
-      <c r="K12" s="38">
-        <v>60</v>
-      </c>
-      <c r="L12" s="38">
-        <v>60</v>
-      </c>
-      <c r="M12" s="38">
-        <v>60</v>
-      </c>
-      <c r="N12" s="38">
+      <c r="K12" s="48">
+        <v>60</v>
+      </c>
+      <c r="L12" s="48">
+        <v>60</v>
+      </c>
+      <c r="M12" s="48">
+        <v>60</v>
+      </c>
+      <c r="N12" s="48">
         <v>60</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="40"/>
+      <c r="B13" s="45"/>
       <c r="C13" s="2" t="s">
         <v>2</v>
       </c>
@@ -1812,16 +1818,16 @@
       <c r="G13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="42"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="38"/>
-      <c r="L13" s="38"/>
-      <c r="M13" s="38"/>
-      <c r="N13" s="38"/>
+      <c r="H13" s="46"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="48"/>
+      <c r="L13" s="48"/>
+      <c r="M13" s="48"/>
+      <c r="N13" s="48"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="40"/>
+      <c r="B14" s="45"/>
       <c r="C14" s="2" t="s">
         <v>23</v>
       </c>
@@ -1833,16 +1839,16 @@
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="42"/>
-      <c r="J14" s="43"/>
-      <c r="K14" s="38"/>
-      <c r="L14" s="38"/>
-      <c r="M14" s="38"/>
-      <c r="N14" s="38"/>
+      <c r="H14" s="46"/>
+      <c r="I14" s="46"/>
+      <c r="J14" s="47"/>
+      <c r="K14" s="48"/>
+      <c r="L14" s="48"/>
+      <c r="M14" s="48"/>
+      <c r="N14" s="48"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="41"/>
+      <c r="B15" s="49"/>
       <c r="C15" s="2" t="s">
         <v>26</v>
       </c>
@@ -1850,26 +1856,16 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="43"/>
-      <c r="K15" s="38"/>
-      <c r="L15" s="38"/>
-      <c r="M15" s="38"/>
-      <c r="N15" s="38"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="46"/>
+      <c r="J15" s="47"/>
+      <c r="K15" s="48"/>
+      <c r="L15" s="48"/>
+      <c r="M15" s="48"/>
+      <c r="N15" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="J4:J7"/>
-    <mergeCell ref="K4:K7"/>
-    <mergeCell ref="L4:L7"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:N2"/>
-    <mergeCell ref="M4:M7"/>
-    <mergeCell ref="N4:N7"/>
-    <mergeCell ref="I4:I7"/>
-    <mergeCell ref="H4:H7"/>
     <mergeCell ref="L12:L15"/>
     <mergeCell ref="M12:M15"/>
     <mergeCell ref="N12:N15"/>
@@ -1886,6 +1882,16 @@
     <mergeCell ref="L8:L11"/>
     <mergeCell ref="M8:M11"/>
     <mergeCell ref="N8:N11"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="J4:J7"/>
+    <mergeCell ref="K4:K7"/>
+    <mergeCell ref="L4:L7"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:N2"/>
+    <mergeCell ref="M4:M7"/>
+    <mergeCell ref="N4:N7"/>
+    <mergeCell ref="I4:I7"/>
+    <mergeCell ref="H4:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1912,40 +1918,40 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="55"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="52"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="47" t="s">
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="48"/>
-      <c r="M3" s="48"/>
-      <c r="N3" s="49"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="43"/>
     </row>
     <row r="4" spans="2:14" ht="33" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
@@ -1989,7 +1995,7 @@
       </c>
     </row>
     <row r="5" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="53" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="11" t="s">
@@ -2003,24 +2009,24 @@
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="17"/>
-      <c r="H5" s="52">
+      <c r="H5" s="56">
         <v>6</v>
       </c>
-      <c r="I5" s="42">
+      <c r="I5" s="46">
         <v>2</v>
       </c>
-      <c r="J5" s="43">
+      <c r="J5" s="47">
         <v>100</v>
       </c>
-      <c r="K5" s="38">
-        <v>60</v>
-      </c>
-      <c r="L5" s="38"/>
-      <c r="M5" s="38"/>
-      <c r="N5" s="38"/>
+      <c r="K5" s="48">
+        <v>60</v>
+      </c>
+      <c r="L5" s="48"/>
+      <c r="M5" s="48"/>
+      <c r="N5" s="48"/>
     </row>
     <row r="6" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="51"/>
+      <c r="B6" s="54"/>
       <c r="C6" s="14" t="s">
         <v>2</v>
       </c>
@@ -2036,16 +2042,16 @@
       <c r="G6" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="52"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="38"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="38"/>
-      <c r="N6" s="38"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="48"/>
+      <c r="N6" s="48"/>
     </row>
     <row r="7" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="53" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="15" t="s">
@@ -2059,22 +2065,22 @@
       </c>
       <c r="F7" s="20"/>
       <c r="G7" s="21"/>
-      <c r="H7" s="52">
+      <c r="H7" s="56">
         <v>8</v>
       </c>
-      <c r="I7" s="42">
-        <v>4</v>
-      </c>
-      <c r="J7" s="43">
+      <c r="I7" s="46">
+        <v>4</v>
+      </c>
+      <c r="J7" s="47">
         <v>100</v>
       </c>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="38"/>
-      <c r="N7" s="38"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="48"/>
+      <c r="M7" s="48"/>
+      <c r="N7" s="48"/>
     </row>
     <row r="8" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="51"/>
+      <c r="B8" s="54"/>
       <c r="C8" s="14" t="s">
         <v>2</v>
       </c>
@@ -2090,16 +2096,16 @@
       <c r="G8" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="52"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="38"/>
-      <c r="L8" s="38"/>
-      <c r="M8" s="38"/>
-      <c r="N8" s="38"/>
+      <c r="H8" s="56"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="48"/>
+      <c r="L8" s="48"/>
+      <c r="M8" s="48"/>
+      <c r="N8" s="48"/>
     </row>
     <row r="9" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="53" t="s">
         <v>36</v>
       </c>
       <c r="C9" s="15" t="s">
@@ -2113,22 +2119,22 @@
       </c>
       <c r="F9" s="20"/>
       <c r="G9" s="21"/>
-      <c r="H9" s="52">
+      <c r="H9" s="56">
         <v>8</v>
       </c>
-      <c r="I9" s="42">
-        <v>4</v>
-      </c>
-      <c r="J9" s="43">
-        <v>60</v>
-      </c>
-      <c r="K9" s="38"/>
-      <c r="L9" s="38"/>
-      <c r="M9" s="38"/>
-      <c r="N9" s="38"/>
+      <c r="I9" s="46">
+        <v>4</v>
+      </c>
+      <c r="J9" s="47">
+        <v>60</v>
+      </c>
+      <c r="K9" s="48"/>
+      <c r="L9" s="48"/>
+      <c r="M9" s="48"/>
+      <c r="N9" s="48"/>
     </row>
     <row r="10" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="51"/>
+      <c r="B10" s="54"/>
       <c r="C10" s="14" t="s">
         <v>2</v>
       </c>
@@ -2144,16 +2150,16 @@
       <c r="G10" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="52"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="38"/>
-      <c r="N10" s="38"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="48"/>
+      <c r="M10" s="48"/>
+      <c r="N10" s="48"/>
     </row>
     <row r="11" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="50" t="s">
+      <c r="B11" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C11" s="15" t="s">
@@ -2167,30 +2173,30 @@
       </c>
       <c r="F11" s="20"/>
       <c r="G11" s="21"/>
-      <c r="H11" s="52">
+      <c r="H11" s="56">
         <v>8</v>
       </c>
-      <c r="I11" s="42">
-        <v>4</v>
-      </c>
-      <c r="J11" s="43">
-        <v>60</v>
-      </c>
-      <c r="K11" s="38">
+      <c r="I11" s="46">
+        <v>4</v>
+      </c>
+      <c r="J11" s="47">
+        <v>60</v>
+      </c>
+      <c r="K11" s="48">
         <v>50</v>
       </c>
-      <c r="L11" s="38">
+      <c r="L11" s="48">
         <v>50</v>
       </c>
-      <c r="M11" s="38">
+      <c r="M11" s="48">
         <v>50</v>
       </c>
-      <c r="N11" s="38">
+      <c r="N11" s="48">
         <v>50</v>
       </c>
     </row>
     <row r="12" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="51"/>
+      <c r="B12" s="54"/>
       <c r="C12" s="15" t="s">
         <v>2</v>
       </c>
@@ -2206,16 +2212,16 @@
       <c r="G12" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="52"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="43"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="38"/>
-      <c r="M12" s="38"/>
-      <c r="N12" s="38"/>
+      <c r="H12" s="56"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="48"/>
+      <c r="L12" s="48"/>
+      <c r="M12" s="48"/>
+      <c r="N12" s="48"/>
     </row>
     <row r="13" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="56"/>
+      <c r="B13" s="55"/>
       <c r="C13" s="14" t="s">
         <v>23</v>
       </c>
@@ -2227,16 +2233,35 @@
       </c>
       <c r="F13" s="24"/>
       <c r="G13" s="25"/>
-      <c r="H13" s="52"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="38"/>
-      <c r="L13" s="38"/>
-      <c r="M13" s="38"/>
-      <c r="N13" s="38"/>
+      <c r="H13" s="56"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="48"/>
+      <c r="L13" s="48"/>
+      <c r="M13" s="48"/>
+      <c r="N13" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="H3:N3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
     <mergeCell ref="M11:M13"/>
     <mergeCell ref="N11:N13"/>
     <mergeCell ref="B2:N2"/>
@@ -2253,25 +2278,6 @@
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
     <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="H3:N3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -2300,40 +2306,40 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="55"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="52"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="47" t="s">
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="48"/>
-      <c r="M3" s="48"/>
-      <c r="N3" s="49"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="43"/>
     </row>
     <row r="4" spans="2:14" ht="33" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
@@ -2377,7 +2383,7 @@
       </c>
     </row>
     <row r="5" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="53" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="26" t="s">
@@ -2391,24 +2397,24 @@
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="17"/>
-      <c r="H5" s="52">
+      <c r="H5" s="56">
         <v>6</v>
       </c>
-      <c r="I5" s="42">
+      <c r="I5" s="46">
         <v>2</v>
       </c>
-      <c r="J5" s="43">
+      <c r="J5" s="47">
         <v>100</v>
       </c>
-      <c r="K5" s="38">
-        <v>60</v>
-      </c>
-      <c r="L5" s="38"/>
-      <c r="M5" s="38"/>
-      <c r="N5" s="38"/>
+      <c r="K5" s="48">
+        <v>60</v>
+      </c>
+      <c r="L5" s="48"/>
+      <c r="M5" s="48"/>
+      <c r="N5" s="48"/>
     </row>
     <row r="6" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="51"/>
+      <c r="B6" s="54"/>
       <c r="C6" s="27" t="s">
         <v>40</v>
       </c>
@@ -2424,16 +2430,16 @@
       <c r="G6" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="52"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="38"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="38"/>
-      <c r="N6" s="38"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="48"/>
+      <c r="N6" s="48"/>
     </row>
     <row r="7" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="53" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="28" t="s">
@@ -2447,22 +2453,22 @@
       </c>
       <c r="F7" s="20"/>
       <c r="G7" s="21"/>
-      <c r="H7" s="52">
+      <c r="H7" s="56">
         <v>8</v>
       </c>
-      <c r="I7" s="42">
-        <v>4</v>
-      </c>
-      <c r="J7" s="43">
+      <c r="I7" s="46">
+        <v>4</v>
+      </c>
+      <c r="J7" s="47">
         <v>100</v>
       </c>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="38"/>
-      <c r="N7" s="38"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="48"/>
+      <c r="M7" s="48"/>
+      <c r="N7" s="48"/>
     </row>
     <row r="8" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="51"/>
+      <c r="B8" s="54"/>
       <c r="C8" s="27" t="s">
         <v>40</v>
       </c>
@@ -2478,16 +2484,16 @@
       <c r="G8" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="52"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="38"/>
-      <c r="L8" s="38"/>
-      <c r="M8" s="38"/>
-      <c r="N8" s="38"/>
+      <c r="H8" s="56"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="48"/>
+      <c r="L8" s="48"/>
+      <c r="M8" s="48"/>
+      <c r="N8" s="48"/>
     </row>
     <row r="9" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="53" t="s">
         <v>36</v>
       </c>
       <c r="C9" s="28" t="s">
@@ -2501,22 +2507,22 @@
       </c>
       <c r="F9" s="20"/>
       <c r="G9" s="21"/>
-      <c r="H9" s="52">
+      <c r="H9" s="56">
         <v>8</v>
       </c>
-      <c r="I9" s="42">
-        <v>4</v>
-      </c>
-      <c r="J9" s="43">
-        <v>60</v>
-      </c>
-      <c r="K9" s="38"/>
-      <c r="L9" s="38"/>
-      <c r="M9" s="38"/>
-      <c r="N9" s="38"/>
+      <c r="I9" s="46">
+        <v>4</v>
+      </c>
+      <c r="J9" s="47">
+        <v>60</v>
+      </c>
+      <c r="K9" s="48"/>
+      <c r="L9" s="48"/>
+      <c r="M9" s="48"/>
+      <c r="N9" s="48"/>
     </row>
     <row r="10" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="51"/>
+      <c r="B10" s="54"/>
       <c r="C10" s="27" t="s">
         <v>40</v>
       </c>
@@ -2532,16 +2538,16 @@
       <c r="G10" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="52"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="38"/>
-      <c r="N10" s="38"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="48"/>
+      <c r="M10" s="48"/>
+      <c r="N10" s="48"/>
     </row>
     <row r="11" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="50" t="s">
+      <c r="B11" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C11" s="28" t="s">
@@ -2555,30 +2561,30 @@
       </c>
       <c r="F11" s="20"/>
       <c r="G11" s="21"/>
-      <c r="H11" s="52">
+      <c r="H11" s="56">
         <v>8</v>
       </c>
-      <c r="I11" s="42">
-        <v>4</v>
-      </c>
-      <c r="J11" s="43">
-        <v>60</v>
-      </c>
-      <c r="K11" s="38">
+      <c r="I11" s="46">
+        <v>4</v>
+      </c>
+      <c r="J11" s="47">
+        <v>60</v>
+      </c>
+      <c r="K11" s="48">
         <v>50</v>
       </c>
-      <c r="L11" s="38">
+      <c r="L11" s="48">
         <v>50</v>
       </c>
-      <c r="M11" s="38">
+      <c r="M11" s="48">
         <v>50</v>
       </c>
-      <c r="N11" s="38">
+      <c r="N11" s="48">
         <v>50</v>
       </c>
     </row>
     <row r="12" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="51"/>
+      <c r="B12" s="54"/>
       <c r="C12" s="29" t="s">
         <v>40</v>
       </c>
@@ -2594,16 +2600,16 @@
       <c r="G12" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="52"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="43"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="38"/>
-      <c r="M12" s="38"/>
-      <c r="N12" s="38"/>
+      <c r="H12" s="56"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="48"/>
+      <c r="L12" s="48"/>
+      <c r="M12" s="48"/>
+      <c r="N12" s="48"/>
     </row>
     <row r="13" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="56"/>
+      <c r="B13" s="55"/>
       <c r="C13" s="30" t="s">
         <v>41</v>
       </c>
@@ -2615,37 +2621,16 @@
       </c>
       <c r="F13" s="24"/>
       <c r="G13" s="25"/>
-      <c r="H13" s="52"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="38"/>
-      <c r="L13" s="38"/>
-      <c r="M13" s="38"/>
-      <c r="N13" s="38"/>
+      <c r="H13" s="56"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="48"/>
+      <c r="L13" s="48"/>
+      <c r="M13" s="48"/>
+      <c r="N13" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="H3:N3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
     <mergeCell ref="L11:L13"/>
     <mergeCell ref="M11:M13"/>
     <mergeCell ref="N11:N13"/>
@@ -2660,6 +2645,27 @@
     <mergeCell ref="I11:I13"/>
     <mergeCell ref="J11:J13"/>
     <mergeCell ref="K11:K13"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="H3:N3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
Cập nhật tài liệu CEPH
</commit_message>
<xml_diff>
--- a/tools/IP-Planning-Hardware-Requirements.xlsx
+++ b/tools/IP-Planning-Hardware-Requirements.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7776" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Luminous-zabbix" sheetId="11" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="77">
   <si>
     <t>Controller</t>
   </si>
@@ -203,15 +203,9 @@
     <t>ens160</t>
   </si>
   <si>
-    <t>192.168.70.1</t>
-  </si>
-  <si>
     <t>+100GB</t>
   </si>
   <si>
-    <t>CEPH COM</t>
-  </si>
-  <si>
     <t>VLAN82</t>
   </si>
   <si>
@@ -221,51 +215,18 @@
     <t>ens224</t>
   </si>
   <si>
-    <t>+80GB</t>
-  </si>
-  <si>
-    <t>192.168.70.131</t>
-  </si>
-  <si>
     <t>+2GB</t>
   </si>
   <si>
-    <t>192.168.82.131</t>
-  </si>
-  <si>
     <t>CEPH REPLICATE</t>
   </si>
   <si>
     <t>VLAN83</t>
   </si>
   <si>
-    <t>192.168.83.131</t>
-  </si>
-  <si>
-    <t>192.168.70.132</t>
-  </si>
-  <si>
-    <t>192.168.82.132</t>
-  </si>
-  <si>
-    <t>192.168.83.132</t>
-  </si>
-  <si>
-    <t>192.168.70.133</t>
-  </si>
-  <si>
-    <t>192.168.82.133</t>
-  </si>
-  <si>
-    <t>192.168.83.133</t>
-  </si>
-  <si>
     <t>Client1</t>
   </si>
   <si>
-    <t>192.168.70.139</t>
-  </si>
-  <si>
     <t>IP PLANNING  - CEPH 03 NODE</t>
   </si>
   <si>
@@ -275,14 +236,41 @@
     <t>+50GB</t>
   </si>
   <si>
-    <t>192.168.82.139</t>
+    <t>CEPH Public</t>
+  </si>
+  <si>
+    <t>192.168.98.85</t>
+  </si>
+  <si>
+    <t>192.168.98.84</t>
+  </si>
+  <si>
+    <t>192.168.62.84</t>
+  </si>
+  <si>
+    <t>192.168.62.85</t>
+  </si>
+  <si>
+    <t>192.168.63.85</t>
+  </si>
+  <si>
+    <t>192.168.98.86</t>
+  </si>
+  <si>
+    <t>192.168.62.86</t>
+  </si>
+  <si>
+    <t>192.168.63.86</t>
+  </si>
+  <si>
+    <t>192.168.98.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -317,15 +305,8 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color rgb="FFFF0000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -370,13 +351,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -544,7 +531,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -634,40 +621,50 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -679,18 +676,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -703,36 +703,17 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1023,40 +1004,40 @@
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="15.7265625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.1796875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="17.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7265625" style="2" customWidth="1"/>
+    <col min="2" max="3" width="15.77734375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.21875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="17.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.77734375" style="2" customWidth="1"/>
     <col min="7" max="7" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.1796875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="6.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.21875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="6.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="26" style="2" customWidth="1"/>
-    <col min="11" max="11" width="28.54296875" style="2" customWidth="1"/>
-    <col min="12" max="14" width="9.54296875" style="2" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="28.5546875" style="2" customWidth="1"/>
+    <col min="12" max="14" width="9.5546875" style="2" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="39" t="s">
+    <row r="2" spans="2:14" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="42" t="s">
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="44"/>
-    </row>
-    <row r="3" spans="2:14" ht="32" x14ac:dyDescent="0.35">
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="39"/>
+    </row>
+    <row r="3" spans="2:14" ht="33.6" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
@@ -1097,8 +1078,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B4" s="34" t="s">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B4" s="40" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="30" t="s">
@@ -1116,30 +1097,30 @@
       <c r="G4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="37">
-        <v>4</v>
-      </c>
-      <c r="I4" s="37">
+      <c r="H4" s="42">
+        <v>4</v>
+      </c>
+      <c r="I4" s="42">
         <v>2</v>
       </c>
-      <c r="J4" s="38">
+      <c r="J4" s="43">
         <v>40</v>
       </c>
-      <c r="K4" s="33">
+      <c r="K4" s="44">
         <v>40</v>
       </c>
-      <c r="L4" s="33">
+      <c r="L4" s="44">
         <v>60</v>
       </c>
-      <c r="M4" s="33">
+      <c r="M4" s="44">
         <v>60</v>
       </c>
-      <c r="N4" s="33">
+      <c r="N4" s="44">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B5" s="35"/>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B5" s="41"/>
       <c r="C5" s="30" t="s">
         <v>2</v>
       </c>
@@ -1151,16 +1132,16 @@
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B6" s="35"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="44"/>
+      <c r="M5" s="44"/>
+      <c r="N5" s="44"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B6" s="41"/>
       <c r="C6" s="30" t="s">
         <v>20</v>
       </c>
@@ -1172,16 +1153,16 @@
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="33"/>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B7" s="34" t="s">
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="44"/>
+      <c r="N6" s="44"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B7" s="40" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="30" t="s">
@@ -1199,30 +1180,30 @@
       <c r="G7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="37">
-        <v>4</v>
-      </c>
-      <c r="I7" s="37">
+      <c r="H7" s="42">
+        <v>4</v>
+      </c>
+      <c r="I7" s="42">
         <v>2</v>
       </c>
-      <c r="J7" s="38">
+      <c r="J7" s="43">
         <v>40</v>
       </c>
-      <c r="K7" s="33">
+      <c r="K7" s="44">
         <v>40</v>
       </c>
-      <c r="L7" s="33">
+      <c r="L7" s="44">
         <v>60</v>
       </c>
-      <c r="M7" s="33">
+      <c r="M7" s="44">
         <v>60</v>
       </c>
-      <c r="N7" s="33">
+      <c r="N7" s="44">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B8" s="35"/>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B8" s="41"/>
       <c r="C8" s="30" t="s">
         <v>2</v>
       </c>
@@ -1234,16 +1215,16 @@
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33"/>
-      <c r="N8" s="33"/>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B9" s="36"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="44"/>
+      <c r="L8" s="44"/>
+      <c r="M8" s="44"/>
+      <c r="N8" s="44"/>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B9" s="45"/>
       <c r="C9" s="30" t="s">
         <v>20</v>
       </c>
@@ -1255,15 +1236,15 @@
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="33"/>
-      <c r="N9" s="33"/>
-    </row>
-    <row r="10" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="44"/>
+      <c r="L9" s="44"/>
+      <c r="M9" s="44"/>
+      <c r="N9" s="44"/>
+    </row>
+    <row r="10" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="32" t="s">
         <v>44</v>
       </c>
@@ -1306,6 +1287,14 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="M7:M9"/>
+    <mergeCell ref="N7:N9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="J7:J9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="L7:L9"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="H2:N2"/>
     <mergeCell ref="B4:B6"/>
@@ -1316,14 +1305,6 @@
     <mergeCell ref="L4:L6"/>
     <mergeCell ref="M4:M6"/>
     <mergeCell ref="N4:N6"/>
-    <mergeCell ref="M7:M9"/>
-    <mergeCell ref="N7:N9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="J7:J9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="L7:L9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="77" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -1341,40 +1322,40 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="15.7265625" style="2" customWidth="1"/>
+    <col min="2" max="3" width="15.77734375" style="2" customWidth="1"/>
     <col min="4" max="4" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7265625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="17.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.77734375" style="2" customWidth="1"/>
     <col min="7" max="7" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.1796875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="6.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.21875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="6.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="26" style="2" customWidth="1"/>
-    <col min="11" max="11" width="28.54296875" style="2" customWidth="1"/>
-    <col min="12" max="14" width="9.54296875" style="2" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="28.5546875" style="2" customWidth="1"/>
+    <col min="12" max="14" width="9.5546875" style="2" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="39" t="s">
+    <row r="2" spans="2:14" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="42" t="s">
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="44"/>
-    </row>
-    <row r="3" spans="2:14" ht="32" x14ac:dyDescent="0.35">
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="39"/>
+    </row>
+    <row r="3" spans="2:14" ht="33.6" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
@@ -1415,8 +1396,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B4" s="34" t="s">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B4" s="40" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="27" t="s">
@@ -1434,30 +1415,30 @@
       <c r="G4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="37">
-        <v>4</v>
-      </c>
-      <c r="I4" s="37">
+      <c r="H4" s="42">
+        <v>4</v>
+      </c>
+      <c r="I4" s="42">
         <v>2</v>
       </c>
-      <c r="J4" s="38">
+      <c r="J4" s="43">
         <v>40</v>
       </c>
-      <c r="K4" s="33">
+      <c r="K4" s="44">
         <v>40</v>
       </c>
-      <c r="L4" s="33">
+      <c r="L4" s="44">
         <v>60</v>
       </c>
-      <c r="M4" s="33">
+      <c r="M4" s="44">
         <v>60</v>
       </c>
-      <c r="N4" s="33">
+      <c r="N4" s="44">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B5" s="35"/>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B5" s="41"/>
       <c r="C5" s="27" t="s">
         <v>2</v>
       </c>
@@ -1469,16 +1450,16 @@
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B6" s="35"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="44"/>
+      <c r="M5" s="44"/>
+      <c r="N5" s="44"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B6" s="41"/>
       <c r="C6" s="27" t="s">
         <v>20</v>
       </c>
@@ -1490,16 +1471,16 @@
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="33"/>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B7" s="34" t="s">
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="44"/>
+      <c r="N6" s="44"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B7" s="40" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="27" t="s">
@@ -1517,30 +1498,30 @@
       <c r="G7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="37">
-        <v>4</v>
-      </c>
-      <c r="I7" s="37">
+      <c r="H7" s="42">
+        <v>4</v>
+      </c>
+      <c r="I7" s="42">
         <v>2</v>
       </c>
-      <c r="J7" s="38">
+      <c r="J7" s="43">
         <v>40</v>
       </c>
-      <c r="K7" s="33">
+      <c r="K7" s="44">
         <v>40</v>
       </c>
-      <c r="L7" s="33">
+      <c r="L7" s="44">
         <v>60</v>
       </c>
-      <c r="M7" s="33">
+      <c r="M7" s="44">
         <v>60</v>
       </c>
-      <c r="N7" s="33">
+      <c r="N7" s="44">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B8" s="35"/>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B8" s="41"/>
       <c r="C8" s="27" t="s">
         <v>2</v>
       </c>
@@ -1552,16 +1533,16 @@
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33"/>
-      <c r="N8" s="33"/>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B9" s="36"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="44"/>
+      <c r="L8" s="44"/>
+      <c r="M8" s="44"/>
+      <c r="N8" s="44"/>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B9" s="45"/>
       <c r="C9" s="27" t="s">
         <v>20</v>
       </c>
@@ -1573,16 +1554,24 @@
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="33"/>
-      <c r="N9" s="33"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="44"/>
+      <c r="L9" s="44"/>
+      <c r="M9" s="44"/>
+      <c r="N9" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="M7:M9"/>
+    <mergeCell ref="N7:N9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="J7:J9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="L7:L9"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="H2:N2"/>
     <mergeCell ref="B4:B6"/>
@@ -1593,14 +1582,6 @@
     <mergeCell ref="L4:L6"/>
     <mergeCell ref="M4:M6"/>
     <mergeCell ref="N4:N6"/>
-    <mergeCell ref="M7:M9"/>
-    <mergeCell ref="N7:N9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="J7:J9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="L7:L9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="78" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -1615,56 +1596,56 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.7265625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" style="2" customWidth="1"/>
     <col min="3" max="3" width="19" style="26" customWidth="1"/>
     <col min="4" max="4" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7265625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="17.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.77734375" style="2" customWidth="1"/>
     <col min="7" max="7" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.1796875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="6.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="14" width="9.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.21875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="6.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="14" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" ht="54.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="48" t="s">
+    <row r="2" spans="2:14" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="50"/>
-    </row>
-    <row r="3" spans="2:14" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="39" t="s">
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="48"/>
+    </row>
+    <row r="3" spans="2:14" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="42" t="s">
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="44"/>
-    </row>
-    <row r="4" spans="2:14" ht="32" x14ac:dyDescent="0.35">
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="39"/>
+    </row>
+    <row r="4" spans="2:14" ht="33.6" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>7</v>
       </c>
@@ -1705,8 +1686,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="45" t="s">
+    <row r="5" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="49" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="21" t="s">
@@ -1720,24 +1701,24 @@
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="12"/>
-      <c r="H5" s="47">
+      <c r="H5" s="51">
         <v>6</v>
       </c>
-      <c r="I5" s="37">
+      <c r="I5" s="42">
         <v>2</v>
       </c>
-      <c r="J5" s="38">
+      <c r="J5" s="43">
         <v>100</v>
       </c>
-      <c r="K5" s="33">
+      <c r="K5" s="44">
         <v>60</v>
       </c>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
-    </row>
-    <row r="6" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="46"/>
+      <c r="L5" s="44"/>
+      <c r="M5" s="44"/>
+      <c r="N5" s="44"/>
+    </row>
+    <row r="6" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="50"/>
       <c r="C6" s="22" t="s">
         <v>36</v>
       </c>
@@ -1753,16 +1734,16 @@
       <c r="G6" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="47"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="33"/>
-    </row>
-    <row r="7" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="45" t="s">
+      <c r="H6" s="51"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="44"/>
+      <c r="N6" s="44"/>
+    </row>
+    <row r="7" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="49" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="23" t="s">
@@ -1776,22 +1757,22 @@
       </c>
       <c r="F7" s="15"/>
       <c r="G7" s="16"/>
-      <c r="H7" s="47">
+      <c r="H7" s="51">
         <v>8</v>
       </c>
-      <c r="I7" s="37">
-        <v>4</v>
-      </c>
-      <c r="J7" s="38">
+      <c r="I7" s="42">
+        <v>4</v>
+      </c>
+      <c r="J7" s="43">
         <v>100</v>
       </c>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="33"/>
-    </row>
-    <row r="8" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="46"/>
+      <c r="K7" s="44"/>
+      <c r="L7" s="44"/>
+      <c r="M7" s="44"/>
+      <c r="N7" s="44"/>
+    </row>
+    <row r="8" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="50"/>
       <c r="C8" s="22" t="s">
         <v>36</v>
       </c>
@@ -1807,16 +1788,16 @@
       <c r="G8" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="47"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33"/>
-      <c r="N8" s="33"/>
-    </row>
-    <row r="9" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="45" t="s">
+      <c r="H8" s="51"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="44"/>
+      <c r="L8" s="44"/>
+      <c r="M8" s="44"/>
+      <c r="N8" s="44"/>
+    </row>
+    <row r="9" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="49" t="s">
         <v>32</v>
       </c>
       <c r="C9" s="23" t="s">
@@ -1830,22 +1811,22 @@
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="16"/>
-      <c r="H9" s="47">
+      <c r="H9" s="51">
         <v>8</v>
       </c>
-      <c r="I9" s="37">
-        <v>4</v>
-      </c>
-      <c r="J9" s="38">
+      <c r="I9" s="42">
+        <v>4</v>
+      </c>
+      <c r="J9" s="43">
         <v>60</v>
       </c>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="33"/>
-      <c r="N9" s="33"/>
-    </row>
-    <row r="10" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="46"/>
+      <c r="K9" s="44"/>
+      <c r="L9" s="44"/>
+      <c r="M9" s="44"/>
+      <c r="N9" s="44"/>
+    </row>
+    <row r="10" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="50"/>
       <c r="C10" s="22" t="s">
         <v>36</v>
       </c>
@@ -1861,16 +1842,16 @@
       <c r="G10" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="47"/>
-      <c r="I10" s="37"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="33"/>
-      <c r="L10" s="33"/>
-      <c r="M10" s="33"/>
-      <c r="N10" s="33"/>
-    </row>
-    <row r="11" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="45" t="s">
+      <c r="H10" s="51"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="44"/>
+      <c r="L10" s="44"/>
+      <c r="M10" s="44"/>
+      <c r="N10" s="44"/>
+    </row>
+    <row r="11" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="49" t="s">
         <v>33</v>
       </c>
       <c r="C11" s="23" t="s">
@@ -1884,30 +1865,30 @@
       </c>
       <c r="F11" s="15"/>
       <c r="G11" s="16"/>
-      <c r="H11" s="47">
+      <c r="H11" s="51">
         <v>8</v>
       </c>
-      <c r="I11" s="37">
-        <v>4</v>
-      </c>
-      <c r="J11" s="38">
+      <c r="I11" s="42">
+        <v>4</v>
+      </c>
+      <c r="J11" s="43">
         <v>60</v>
       </c>
-      <c r="K11" s="33">
+      <c r="K11" s="44">
         <v>50</v>
       </c>
-      <c r="L11" s="33">
+      <c r="L11" s="44">
         <v>50</v>
       </c>
-      <c r="M11" s="33">
+      <c r="M11" s="44">
         <v>50</v>
       </c>
-      <c r="N11" s="33">
+      <c r="N11" s="44">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="46"/>
+    <row r="12" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="50"/>
       <c r="C12" s="24" t="s">
         <v>36</v>
       </c>
@@ -1923,16 +1904,16 @@
       <c r="G12" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="47"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="33"/>
-      <c r="L12" s="33"/>
-      <c r="M12" s="33"/>
-      <c r="N12" s="33"/>
-    </row>
-    <row r="13" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="51"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="44"/>
+      <c r="L12" s="44"/>
+      <c r="M12" s="44"/>
+      <c r="N12" s="44"/>
+    </row>
+    <row r="13" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="52"/>
       <c r="C13" s="25" t="s">
         <v>37</v>
       </c>
@@ -1944,37 +1925,16 @@
       </c>
       <c r="F13" s="19"/>
       <c r="G13" s="20"/>
-      <c r="H13" s="47"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="38"/>
-      <c r="K13" s="33"/>
-      <c r="L13" s="33"/>
-      <c r="M13" s="33"/>
-      <c r="N13" s="33"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="44"/>
+      <c r="L13" s="44"/>
+      <c r="M13" s="44"/>
+      <c r="N13" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="H3:N3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
     <mergeCell ref="L11:L13"/>
     <mergeCell ref="M11:M13"/>
     <mergeCell ref="N11:N13"/>
@@ -1989,6 +1949,27 @@
     <mergeCell ref="I11:I13"/>
     <mergeCell ref="J11:J13"/>
     <mergeCell ref="K11:K13"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="H3:N3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -2003,84 +1984,84 @@
   <dimension ref="B2:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.08984375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.26953125" style="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.7265625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="6.90625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.21875" style="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.77734375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="6.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="9.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.77734375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" ht="22" x14ac:dyDescent="0.35">
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
-    </row>
-    <row r="3" spans="2:16" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="53" t="s">
-        <v>77</v>
-      </c>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="53"/>
-      <c r="P3" s="53"/>
-    </row>
-    <row r="4" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="54" t="s">
+    <row r="2" spans="2:16" ht="22.2" x14ac:dyDescent="0.3">
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+    </row>
+    <row r="3" spans="2:16" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="58" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="58"/>
+      <c r="N3" s="58"/>
+      <c r="O3" s="58"/>
+      <c r="P3" s="58"/>
+    </row>
+    <row r="4" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="55" t="s">
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="55"/>
-      <c r="L4" s="55"/>
-      <c r="M4" s="55"/>
-      <c r="N4" s="55"/>
-      <c r="O4" s="55"/>
-      <c r="P4" s="55"/>
-    </row>
-    <row r="5" spans="2:16" ht="32" x14ac:dyDescent="0.35">
+      <c r="K4" s="60"/>
+      <c r="L4" s="60"/>
+      <c r="M4" s="60"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="60"/>
+      <c r="P4" s="60"/>
+    </row>
+    <row r="5" spans="2:16" ht="50.4" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
@@ -2127,372 +2108,392 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="2:16" s="62" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="56" t="s">
+    <row r="6" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="54" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="61" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="61" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="61" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" s="61" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="61" t="s">
+        <v>76</v>
+      </c>
+      <c r="I6" s="61" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="K6" s="42">
+        <v>1</v>
+      </c>
+      <c r="L6" s="56" t="s">
+        <v>66</v>
+      </c>
+      <c r="M6" s="44"/>
+      <c r="N6" s="44"/>
+      <c r="O6" s="44"/>
+      <c r="P6" s="44"/>
+    </row>
+    <row r="7" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="54"/>
+      <c r="C7" s="64" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="64" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="64" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="64" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" s="64" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="64"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="43"/>
+      <c r="M7" s="44"/>
+      <c r="N7" s="44"/>
+      <c r="O7" s="44"/>
+      <c r="P7" s="44"/>
+    </row>
+    <row r="8" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="54" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="61" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="61" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="61" t="s">
+        <v>68</v>
+      </c>
+      <c r="G8" s="61" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="61" t="s">
+        <v>76</v>
+      </c>
+      <c r="I8" s="61" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="K8" s="42">
+        <v>2</v>
+      </c>
+      <c r="L8" s="56" t="s">
+        <v>66</v>
+      </c>
+      <c r="M8" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="N8" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="O8" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="P8" s="44"/>
+    </row>
+    <row r="9" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="54"/>
+      <c r="C9" s="64" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="64" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="64" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="64" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" s="64" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="64"/>
+      <c r="I9" s="64"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="43"/>
+      <c r="M9" s="44"/>
+      <c r="N9" s="44"/>
+      <c r="O9" s="44"/>
+      <c r="P9" s="44"/>
+    </row>
+    <row r="10" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="54"/>
+      <c r="C10" s="63" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="63" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="63" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="63" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="63"/>
+      <c r="I10" s="63"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="44"/>
+      <c r="N10" s="44"/>
+      <c r="O10" s="44"/>
+      <c r="P10" s="44"/>
+    </row>
+    <row r="11" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="54" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="61" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="61" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="61" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" s="61" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="61" t="s">
+        <v>76</v>
+      </c>
+      <c r="I11" s="61" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="K11" s="42">
+        <v>2</v>
+      </c>
+      <c r="L11" s="56" t="s">
+        <v>66</v>
+      </c>
+      <c r="M11" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="N11" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="O11" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="P11" s="44"/>
+    </row>
+    <row r="12" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="54"/>
+      <c r="C12" s="64" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="64" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="64" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="64" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" s="64" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" s="64"/>
+      <c r="I12" s="64"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="43"/>
+      <c r="M12" s="44"/>
+      <c r="N12" s="44"/>
+      <c r="O12" s="44"/>
+      <c r="P12" s="44"/>
+    </row>
+    <row r="13" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="54"/>
+      <c r="C13" s="63" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="63" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="63" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="57" t="s">
+      <c r="G13" s="63" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" s="63"/>
+      <c r="I13" s="63"/>
+      <c r="J13" s="42"/>
+      <c r="K13" s="42"/>
+      <c r="L13" s="43"/>
+      <c r="M13" s="44"/>
+      <c r="N13" s="44"/>
+      <c r="O13" s="44"/>
+      <c r="P13" s="44"/>
+    </row>
+    <row r="14" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="57" t="s">
+      <c r="D14" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="57" t="s">
+      <c r="E14" s="61" t="s">
         <v>55</v>
       </c>
-      <c r="F6" s="58" t="s">
+      <c r="F14" s="61" t="s">
+        <v>73</v>
+      </c>
+      <c r="G14" s="61" t="s">
+        <v>4</v>
+      </c>
+      <c r="H14" s="61" t="s">
         <v>76</v>
       </c>
-      <c r="G6" s="57" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="57" t="s">
+      <c r="I14" s="61" t="s">
+        <v>23</v>
+      </c>
+      <c r="J14" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="K14" s="42">
+        <v>2</v>
+      </c>
+      <c r="L14" s="56" t="s">
+        <v>66</v>
+      </c>
+      <c r="M14" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="I6" s="57" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6" s="59" t="s">
-        <v>78</v>
-      </c>
-      <c r="K6" s="37">
-        <v>1</v>
-      </c>
-      <c r="L6" s="60" t="s">
-        <v>79</v>
-      </c>
-      <c r="M6" s="33"/>
-      <c r="N6" s="33"/>
-      <c r="O6" s="33"/>
-      <c r="P6" s="33"/>
-    </row>
-    <row r="7" spans="2:16" s="62" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="56"/>
-      <c r="C7" s="63" t="s">
+      <c r="N14" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="O14" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="P14" s="44"/>
+    </row>
+    <row r="15" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="54"/>
+      <c r="C15" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="62" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="D7" s="63" t="s">
+      <c r="F15" s="62" t="s">
+        <v>74</v>
+      </c>
+      <c r="G15" s="62" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" s="62"/>
+      <c r="I15" s="62"/>
+      <c r="J15" s="42"/>
+      <c r="K15" s="42"/>
+      <c r="L15" s="43"/>
+      <c r="M15" s="44"/>
+      <c r="N15" s="44"/>
+      <c r="O15" s="44"/>
+      <c r="P15" s="44"/>
+    </row>
+    <row r="16" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="54"/>
+      <c r="C16" s="63" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="63" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="63" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="63" t="s">
-        <v>60</v>
-      </c>
-      <c r="F7" s="64" t="s">
-        <v>80</v>
-      </c>
-      <c r="G7" s="63" t="s">
-        <v>4</v>
-      </c>
-      <c r="H7" s="63"/>
-      <c r="I7" s="63"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="33"/>
-      <c r="O7" s="33"/>
-      <c r="P7" s="33"/>
-    </row>
-    <row r="8" spans="2:16" s="62" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="56" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="57" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="57" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="F8" s="58" t="s">
-        <v>63</v>
-      </c>
-      <c r="G8" s="57" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="I8" s="57" t="s">
-        <v>23</v>
-      </c>
-      <c r="J8" s="59" t="s">
-        <v>64</v>
-      </c>
-      <c r="K8" s="37">
-        <v>2</v>
-      </c>
-      <c r="L8" s="60" t="s">
-        <v>62</v>
-      </c>
-      <c r="M8" s="61" t="s">
-        <v>57</v>
-      </c>
-      <c r="N8" s="61" t="s">
-        <v>57</v>
-      </c>
-      <c r="O8" s="61" t="s">
-        <v>57</v>
-      </c>
-      <c r="P8" s="33"/>
-    </row>
-    <row r="9" spans="2:16" s="62" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="56"/>
-      <c r="C9" s="63" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" s="63" t="s">
-        <v>59</v>
-      </c>
-      <c r="E9" s="63" t="s">
-        <v>60</v>
-      </c>
-      <c r="F9" s="64" t="s">
-        <v>65</v>
-      </c>
-      <c r="G9" s="63" t="s">
-        <v>4</v>
-      </c>
-      <c r="H9" s="63"/>
-      <c r="I9" s="63"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="37"/>
-      <c r="L9" s="38"/>
-      <c r="M9" s="33"/>
-      <c r="N9" s="33"/>
-      <c r="O9" s="33"/>
-      <c r="P9" s="33"/>
-    </row>
-    <row r="10" spans="2:16" s="62" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="56"/>
-      <c r="C10" s="65" t="s">
-        <v>66</v>
-      </c>
-      <c r="D10" s="65" t="s">
-        <v>67</v>
-      </c>
-      <c r="E10" s="65" t="s">
-        <v>61</v>
-      </c>
-      <c r="F10" s="66" t="s">
-        <v>68</v>
-      </c>
-      <c r="G10" s="65" t="s">
-        <v>4</v>
-      </c>
-      <c r="H10" s="65"/>
-      <c r="I10" s="65"/>
-      <c r="J10" s="37"/>
-      <c r="K10" s="37"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="33"/>
-      <c r="N10" s="33"/>
-      <c r="O10" s="33"/>
-      <c r="P10" s="33"/>
-    </row>
-    <row r="11" spans="2:16" s="62" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="56" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="57" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="57" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" s="58" t="s">
-        <v>69</v>
-      </c>
-      <c r="G11" s="57" t="s">
-        <v>4</v>
-      </c>
-      <c r="H11" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="I11" s="57" t="s">
-        <v>23</v>
-      </c>
-      <c r="J11" s="59" t="s">
-        <v>64</v>
-      </c>
-      <c r="K11" s="37">
-        <v>2</v>
-      </c>
-      <c r="L11" s="60" t="s">
-        <v>62</v>
-      </c>
-      <c r="M11" s="61" t="s">
-        <v>57</v>
-      </c>
-      <c r="N11" s="61" t="s">
-        <v>57</v>
-      </c>
-      <c r="O11" s="61" t="s">
-        <v>57</v>
-      </c>
-      <c r="P11" s="33"/>
-    </row>
-    <row r="12" spans="2:16" s="62" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="56"/>
-      <c r="C12" s="63" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" s="63" t="s">
-        <v>59</v>
-      </c>
-      <c r="E12" s="63" t="s">
-        <v>60</v>
-      </c>
-      <c r="F12" s="64" t="s">
-        <v>70</v>
-      </c>
-      <c r="G12" s="63" t="s">
-        <v>4</v>
-      </c>
-      <c r="H12" s="63"/>
-      <c r="I12" s="63"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="37"/>
-      <c r="L12" s="38"/>
-      <c r="M12" s="33"/>
-      <c r="N12" s="33"/>
-      <c r="O12" s="33"/>
-      <c r="P12" s="33"/>
-    </row>
-    <row r="13" spans="2:16" s="62" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="56"/>
-      <c r="C13" s="65" t="s">
-        <v>66</v>
-      </c>
-      <c r="D13" s="65" t="s">
-        <v>67</v>
-      </c>
-      <c r="E13" s="65" t="s">
-        <v>61</v>
-      </c>
-      <c r="F13" s="66" t="s">
-        <v>71</v>
-      </c>
-      <c r="G13" s="65" t="s">
-        <v>4</v>
-      </c>
-      <c r="H13" s="65"/>
-      <c r="I13" s="65"/>
-      <c r="J13" s="37"/>
-      <c r="K13" s="37"/>
-      <c r="L13" s="38"/>
-      <c r="M13" s="33"/>
-      <c r="N13" s="33"/>
-      <c r="O13" s="33"/>
-      <c r="P13" s="33"/>
-    </row>
-    <row r="14" spans="2:16" s="62" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="56" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="57" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="57" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="F14" s="58" t="s">
-        <v>72</v>
-      </c>
-      <c r="G14" s="57" t="s">
-        <v>4</v>
-      </c>
-      <c r="H14" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="I14" s="57" t="s">
-        <v>23</v>
-      </c>
-      <c r="J14" s="59" t="s">
-        <v>64</v>
-      </c>
-      <c r="K14" s="37">
-        <v>2</v>
-      </c>
-      <c r="L14" s="60" t="s">
-        <v>62</v>
-      </c>
-      <c r="M14" s="61" t="s">
-        <v>57</v>
-      </c>
-      <c r="N14" s="61" t="s">
-        <v>57</v>
-      </c>
-      <c r="O14" s="61" t="s">
-        <v>57</v>
-      </c>
-      <c r="P14" s="33"/>
-    </row>
-    <row r="15" spans="2:16" s="62" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="56"/>
-      <c r="C15" s="63" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" s="63" t="s">
-        <v>59</v>
-      </c>
-      <c r="E15" s="63" t="s">
-        <v>60</v>
-      </c>
-      <c r="F15" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="G15" s="63" t="s">
-        <v>4</v>
-      </c>
-      <c r="H15" s="63"/>
-      <c r="I15" s="63"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="37"/>
-      <c r="L15" s="38"/>
-      <c r="M15" s="33"/>
-      <c r="N15" s="33"/>
-      <c r="O15" s="33"/>
-      <c r="P15" s="33"/>
-    </row>
-    <row r="16" spans="2:16" s="62" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="56"/>
-      <c r="C16" s="65" t="s">
-        <v>66</v>
-      </c>
-      <c r="D16" s="65" t="s">
-        <v>67</v>
-      </c>
-      <c r="E16" s="65" t="s">
-        <v>61</v>
-      </c>
-      <c r="F16" s="66" t="s">
-        <v>74</v>
-      </c>
-      <c r="G16" s="65" t="s">
-        <v>4</v>
-      </c>
-      <c r="H16" s="65"/>
-      <c r="I16" s="65"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="37"/>
-      <c r="L16" s="38"/>
-      <c r="M16" s="33"/>
-      <c r="N16" s="33"/>
-      <c r="O16" s="33"/>
-      <c r="P16" s="33"/>
-    </row>
-    <row r="17" ht="20" customHeight="1" x14ac:dyDescent="0.35"/>
+      <c r="F16" s="63" t="s">
+        <v>75</v>
+      </c>
+      <c r="G16" s="63" t="s">
+        <v>4</v>
+      </c>
+      <c r="H16" s="63"/>
+      <c r="I16" s="63"/>
+      <c r="J16" s="42"/>
+      <c r="K16" s="42"/>
+      <c r="L16" s="43"/>
+      <c r="M16" s="44"/>
+      <c r="N16" s="44"/>
+      <c r="O16" s="44"/>
+      <c r="P16" s="44"/>
+    </row>
+    <row r="17" ht="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="B2:P2"/>
+    <mergeCell ref="B3:P3"/>
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="J4:P4"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="P6:P7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="J8:J10"/>
+    <mergeCell ref="K8:K10"/>
+    <mergeCell ref="L8:L10"/>
+    <mergeCell ref="M8:M10"/>
+    <mergeCell ref="N8:N10"/>
+    <mergeCell ref="O8:O10"/>
+    <mergeCell ref="P8:P10"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N6:N7"/>
     <mergeCell ref="O11:O13"/>
     <mergeCell ref="P11:P13"/>
     <mergeCell ref="B14:B16"/>
@@ -2509,26 +2510,6 @@
     <mergeCell ref="L11:L13"/>
     <mergeCell ref="M11:M13"/>
     <mergeCell ref="N11:N13"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="P6:P7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="J8:J10"/>
-    <mergeCell ref="K8:K10"/>
-    <mergeCell ref="L8:L10"/>
-    <mergeCell ref="M8:M10"/>
-    <mergeCell ref="N8:N10"/>
-    <mergeCell ref="O8:O10"/>
-    <mergeCell ref="P8:P10"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="B2:P2"/>
-    <mergeCell ref="B3:P3"/>
-    <mergeCell ref="B4:I4"/>
-    <mergeCell ref="J4:P4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="61" fitToHeight="0" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
update topo & ip planning
</commit_message>
<xml_diff>
--- a/tools/IP-Planning-Hardware-Requirements.xlsx
+++ b/tools/IP-Planning-Hardware-Requirements.xlsx
@@ -197,24 +197,12 @@
     <t>MGNT</t>
   </si>
   <si>
-    <t>VLAN70</t>
-  </si>
-  <si>
-    <t>ens160</t>
-  </si>
-  <si>
     <t>+100GB</t>
   </si>
   <si>
     <t>VLAN82</t>
   </si>
   <si>
-    <t>ens192</t>
-  </si>
-  <si>
-    <t>ens224</t>
-  </si>
-  <si>
     <t>+2GB</t>
   </si>
   <si>
@@ -239,31 +227,43 @@
     <t>CEPH Public</t>
   </si>
   <si>
-    <t>192.168.98.85</t>
-  </si>
-  <si>
-    <t>192.168.98.84</t>
-  </si>
-  <si>
-    <t>192.168.62.84</t>
-  </si>
-  <si>
-    <t>192.168.62.85</t>
-  </si>
-  <si>
-    <t>192.168.63.85</t>
-  </si>
-  <si>
-    <t>192.168.98.86</t>
-  </si>
-  <si>
-    <t>192.168.62.86</t>
-  </si>
-  <si>
-    <t>192.168.63.86</t>
-  </si>
-  <si>
-    <t>192.168.98.1</t>
+    <t>VLAN80</t>
+  </si>
+  <si>
+    <t>192.168.80.139</t>
+  </si>
+  <si>
+    <t>192.168.82.139</t>
+  </si>
+  <si>
+    <t>192.168.80.131</t>
+  </si>
+  <si>
+    <t>192.168.80.1</t>
+  </si>
+  <si>
+    <t>192.168.82.131</t>
+  </si>
+  <si>
+    <t>192.168.83.131</t>
+  </si>
+  <si>
+    <t>192.168.80.132</t>
+  </si>
+  <si>
+    <t>192.168.82.132</t>
+  </si>
+  <si>
+    <t>192.168.83.132</t>
+  </si>
+  <si>
+    <t>192.168.82.133</t>
+  </si>
+  <si>
+    <t>192.168.80.133</t>
+  </si>
+  <si>
+    <t>192.168.83.133</t>
   </si>
 </sst>
 </file>
@@ -531,7 +531,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -622,6 +622,33 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -640,22 +667,16 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -667,52 +688,28 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1019,23 +1016,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="37" t="s">
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="39"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="48"/>
     </row>
     <row r="3" spans="2:14" ht="33.6" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
@@ -1079,7 +1076,7 @@
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="38" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="30" t="s">
@@ -1097,30 +1094,30 @@
       <c r="G4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="42">
-        <v>4</v>
-      </c>
-      <c r="I4" s="42">
+      <c r="H4" s="41">
+        <v>4</v>
+      </c>
+      <c r="I4" s="41">
         <v>2</v>
       </c>
-      <c r="J4" s="43">
+      <c r="J4" s="42">
         <v>40</v>
       </c>
-      <c r="K4" s="44">
+      <c r="K4" s="37">
         <v>40</v>
       </c>
-      <c r="L4" s="44">
+      <c r="L4" s="37">
         <v>60</v>
       </c>
-      <c r="M4" s="44">
+      <c r="M4" s="37">
         <v>60</v>
       </c>
-      <c r="N4" s="44">
+      <c r="N4" s="37">
         <v>60</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B5" s="41"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="30" t="s">
         <v>2</v>
       </c>
@@ -1132,16 +1129,16 @@
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
-      <c r="M5" s="44"/>
-      <c r="N5" s="44"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="37"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B6" s="41"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="30" t="s">
         <v>20</v>
       </c>
@@ -1153,16 +1150,16 @@
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="44"/>
-      <c r="L6" s="44"/>
-      <c r="M6" s="44"/>
-      <c r="N6" s="44"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="38" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="30" t="s">
@@ -1180,30 +1177,30 @@
       <c r="G7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="42">
-        <v>4</v>
-      </c>
-      <c r="I7" s="42">
+      <c r="H7" s="41">
+        <v>4</v>
+      </c>
+      <c r="I7" s="41">
         <v>2</v>
       </c>
-      <c r="J7" s="43">
+      <c r="J7" s="42">
         <v>40</v>
       </c>
-      <c r="K7" s="44">
+      <c r="K7" s="37">
         <v>40</v>
       </c>
-      <c r="L7" s="44">
+      <c r="L7" s="37">
         <v>60</v>
       </c>
-      <c r="M7" s="44">
+      <c r="M7" s="37">
         <v>60</v>
       </c>
-      <c r="N7" s="44">
+      <c r="N7" s="37">
         <v>60</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="41"/>
+      <c r="B8" s="39"/>
       <c r="C8" s="30" t="s">
         <v>2</v>
       </c>
@@ -1215,16 +1212,16 @@
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="44"/>
-      <c r="L8" s="44"/>
-      <c r="M8" s="44"/>
-      <c r="N8" s="44"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="37"/>
+      <c r="N8" s="37"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="45"/>
+      <c r="B9" s="40"/>
       <c r="C9" s="30" t="s">
         <v>20</v>
       </c>
@@ -1236,13 +1233,13 @@
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="44"/>
-      <c r="L9" s="44"/>
-      <c r="M9" s="44"/>
-      <c r="N9" s="44"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
     </row>
     <row r="10" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="32" t="s">
@@ -1287,14 +1284,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="M7:M9"/>
-    <mergeCell ref="N7:N9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="J7:J9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="L7:L9"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="H2:N2"/>
     <mergeCell ref="B4:B6"/>
@@ -1305,6 +1294,14 @@
     <mergeCell ref="L4:L6"/>
     <mergeCell ref="M4:M6"/>
     <mergeCell ref="N4:N6"/>
+    <mergeCell ref="M7:M9"/>
+    <mergeCell ref="N7:N9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="J7:J9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="L7:L9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="77" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -1337,23 +1334,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="37" t="s">
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="39"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="48"/>
     </row>
     <row r="3" spans="2:14" ht="33.6" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
@@ -1397,7 +1394,7 @@
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="38" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="27" t="s">
@@ -1415,30 +1412,30 @@
       <c r="G4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="42">
-        <v>4</v>
-      </c>
-      <c r="I4" s="42">
+      <c r="H4" s="41">
+        <v>4</v>
+      </c>
+      <c r="I4" s="41">
         <v>2</v>
       </c>
-      <c r="J4" s="43">
+      <c r="J4" s="42">
         <v>40</v>
       </c>
-      <c r="K4" s="44">
+      <c r="K4" s="37">
         <v>40</v>
       </c>
-      <c r="L4" s="44">
+      <c r="L4" s="37">
         <v>60</v>
       </c>
-      <c r="M4" s="44">
+      <c r="M4" s="37">
         <v>60</v>
       </c>
-      <c r="N4" s="44">
+      <c r="N4" s="37">
         <v>60</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B5" s="41"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="27" t="s">
         <v>2</v>
       </c>
@@ -1450,16 +1447,16 @@
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
-      <c r="M5" s="44"/>
-      <c r="N5" s="44"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="37"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B6" s="41"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="27" t="s">
         <v>20</v>
       </c>
@@ -1471,16 +1468,16 @@
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="44"/>
-      <c r="L6" s="44"/>
-      <c r="M6" s="44"/>
-      <c r="N6" s="44"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="38" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="27" t="s">
@@ -1498,30 +1495,30 @@
       <c r="G7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="42">
-        <v>4</v>
-      </c>
-      <c r="I7" s="42">
+      <c r="H7" s="41">
+        <v>4</v>
+      </c>
+      <c r="I7" s="41">
         <v>2</v>
       </c>
-      <c r="J7" s="43">
+      <c r="J7" s="42">
         <v>40</v>
       </c>
-      <c r="K7" s="44">
+      <c r="K7" s="37">
         <v>40</v>
       </c>
-      <c r="L7" s="44">
+      <c r="L7" s="37">
         <v>60</v>
       </c>
-      <c r="M7" s="44">
+      <c r="M7" s="37">
         <v>60</v>
       </c>
-      <c r="N7" s="44">
+      <c r="N7" s="37">
         <v>60</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="41"/>
+      <c r="B8" s="39"/>
       <c r="C8" s="27" t="s">
         <v>2</v>
       </c>
@@ -1533,16 +1530,16 @@
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="44"/>
-      <c r="L8" s="44"/>
-      <c r="M8" s="44"/>
-      <c r="N8" s="44"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="37"/>
+      <c r="N8" s="37"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="45"/>
+      <c r="B9" s="40"/>
       <c r="C9" s="27" t="s">
         <v>20</v>
       </c>
@@ -1554,24 +1551,16 @@
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="44"/>
-      <c r="L9" s="44"/>
-      <c r="M9" s="44"/>
-      <c r="N9" s="44"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="M7:M9"/>
-    <mergeCell ref="N7:N9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="J7:J9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="L7:L9"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="H2:N2"/>
     <mergeCell ref="B4:B6"/>
@@ -1582,6 +1571,14 @@
     <mergeCell ref="L4:L6"/>
     <mergeCell ref="M4:M6"/>
     <mergeCell ref="N4:N6"/>
+    <mergeCell ref="M7:M9"/>
+    <mergeCell ref="N7:N9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="J7:J9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="L7:L9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="78" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -1610,40 +1607,40 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="48"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="55"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="37" t="s">
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="39"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="48"/>
     </row>
     <row r="4" spans="2:14" ht="33.6" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
@@ -1704,18 +1701,18 @@
       <c r="H5" s="51">
         <v>6</v>
       </c>
-      <c r="I5" s="42">
+      <c r="I5" s="41">
         <v>2</v>
       </c>
-      <c r="J5" s="43">
+      <c r="J5" s="42">
         <v>100</v>
       </c>
-      <c r="K5" s="44">
+      <c r="K5" s="37">
         <v>60</v>
       </c>
-      <c r="L5" s="44"/>
-      <c r="M5" s="44"/>
-      <c r="N5" s="44"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="37"/>
     </row>
     <row r="6" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="50"/>
@@ -1735,12 +1732,12 @@
         <v>23</v>
       </c>
       <c r="H6" s="51"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="44"/>
-      <c r="L6" s="44"/>
-      <c r="M6" s="44"/>
-      <c r="N6" s="44"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
     </row>
     <row r="7" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="49" t="s">
@@ -1760,16 +1757,16 @@
       <c r="H7" s="51">
         <v>8</v>
       </c>
-      <c r="I7" s="42">
-        <v>4</v>
-      </c>
-      <c r="J7" s="43">
+      <c r="I7" s="41">
+        <v>4</v>
+      </c>
+      <c r="J7" s="42">
         <v>100</v>
       </c>
-      <c r="K7" s="44"/>
-      <c r="L7" s="44"/>
-      <c r="M7" s="44"/>
-      <c r="N7" s="44"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="37"/>
     </row>
     <row r="8" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="50"/>
@@ -1789,12 +1786,12 @@
         <v>23</v>
       </c>
       <c r="H8" s="51"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="44"/>
-      <c r="L8" s="44"/>
-      <c r="M8" s="44"/>
-      <c r="N8" s="44"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="37"/>
+      <c r="N8" s="37"/>
     </row>
     <row r="9" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="49" t="s">
@@ -1814,16 +1811,16 @@
       <c r="H9" s="51">
         <v>8</v>
       </c>
-      <c r="I9" s="42">
-        <v>4</v>
-      </c>
-      <c r="J9" s="43">
+      <c r="I9" s="41">
+        <v>4</v>
+      </c>
+      <c r="J9" s="42">
         <v>60</v>
       </c>
-      <c r="K9" s="44"/>
-      <c r="L9" s="44"/>
-      <c r="M9" s="44"/>
-      <c r="N9" s="44"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
     </row>
     <row r="10" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="50"/>
@@ -1843,12 +1840,12 @@
         <v>23</v>
       </c>
       <c r="H10" s="51"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="44"/>
-      <c r="L10" s="44"/>
-      <c r="M10" s="44"/>
-      <c r="N10" s="44"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="37"/>
+      <c r="M10" s="37"/>
+      <c r="N10" s="37"/>
     </row>
     <row r="11" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="49" t="s">
@@ -1868,22 +1865,22 @@
       <c r="H11" s="51">
         <v>8</v>
       </c>
-      <c r="I11" s="42">
-        <v>4</v>
-      </c>
-      <c r="J11" s="43">
+      <c r="I11" s="41">
+        <v>4</v>
+      </c>
+      <c r="J11" s="42">
         <v>60</v>
       </c>
-      <c r="K11" s="44">
+      <c r="K11" s="37">
         <v>50</v>
       </c>
-      <c r="L11" s="44">
+      <c r="L11" s="37">
         <v>50</v>
       </c>
-      <c r="M11" s="44">
+      <c r="M11" s="37">
         <v>50</v>
       </c>
-      <c r="N11" s="44">
+      <c r="N11" s="37">
         <v>50</v>
       </c>
     </row>
@@ -1905,12 +1902,12 @@
         <v>23</v>
       </c>
       <c r="H12" s="51"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="43"/>
-      <c r="K12" s="44"/>
-      <c r="L12" s="44"/>
-      <c r="M12" s="44"/>
-      <c r="N12" s="44"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="37"/>
+      <c r="N12" s="37"/>
     </row>
     <row r="13" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="52"/>
@@ -1926,15 +1923,36 @@
       <c r="F13" s="19"/>
       <c r="G13" s="20"/>
       <c r="H13" s="51"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="44"/>
-      <c r="L13" s="44"/>
-      <c r="M13" s="44"/>
-      <c r="N13" s="44"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="42"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="37"/>
+      <c r="M13" s="37"/>
+      <c r="N13" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="H3:N3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
     <mergeCell ref="L11:L13"/>
     <mergeCell ref="M11:M13"/>
     <mergeCell ref="N11:N13"/>
@@ -1949,27 +1967,6 @@
     <mergeCell ref="I11:I13"/>
     <mergeCell ref="J11:J13"/>
     <mergeCell ref="K11:K13"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="H3:N3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -1983,8 +1980,8 @@
   </sheetPr>
   <dimension ref="B2:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
@@ -2005,61 +2002,61 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="22.2" x14ac:dyDescent="0.3">
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57"/>
-      <c r="N2" s="57"/>
-      <c r="O2" s="57"/>
-      <c r="P2" s="57"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="56"/>
+      <c r="P2" s="56"/>
     </row>
     <row r="3" spans="2:16" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="58" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
-      <c r="I3" s="58"/>
-      <c r="J3" s="58"/>
-      <c r="K3" s="58"/>
-      <c r="L3" s="58"/>
-      <c r="M3" s="58"/>
-      <c r="N3" s="58"/>
-      <c r="O3" s="58"/>
-      <c r="P3" s="58"/>
+      <c r="B3" s="57" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="57"/>
+      <c r="P3" s="57"/>
     </row>
     <row r="4" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="60" t="s">
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="58"/>
+      <c r="J4" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60"/>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60"/>
-      <c r="O4" s="60"/>
-      <c r="P4" s="60"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="59"/>
+      <c r="N4" s="59"/>
+      <c r="O4" s="59"/>
+      <c r="P4" s="59"/>
     </row>
     <row r="5" spans="2:16" ht="50.4" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
@@ -2109,391 +2106,371 @@
       </c>
     </row>
     <row r="6" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="54" t="s">
+      <c r="B6" s="60" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="I6" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="K6" s="41">
+        <v>1</v>
+      </c>
+      <c r="L6" s="62" t="s">
+        <v>62</v>
+      </c>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
+      <c r="O6" s="37"/>
+      <c r="P6" s="37"/>
+    </row>
+    <row r="7" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="60"/>
+      <c r="C7" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="61" t="s">
+      <c r="D7" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="G7" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="37"/>
+      <c r="O7" s="37"/>
+      <c r="P7" s="37"/>
+    </row>
+    <row r="8" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="60" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="61" t="s">
+      <c r="D8" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="I8" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="K8" s="41">
+        <v>2</v>
+      </c>
+      <c r="L8" s="62" t="s">
+        <v>62</v>
+      </c>
+      <c r="M8" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="61" t="s">
+      <c r="N8" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="O8" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="P8" s="37"/>
+    </row>
+    <row r="9" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="60"/>
+      <c r="C9" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="F6" s="61" t="s">
+      <c r="E9" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="G6" s="61" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="61" t="s">
+      <c r="G9" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
+      <c r="O9" s="37"/>
+      <c r="P9" s="37"/>
+    </row>
+    <row r="10" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="60"/>
+      <c r="C10" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="35"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="37"/>
+      <c r="N10" s="37"/>
+      <c r="O10" s="37"/>
+      <c r="P10" s="37"/>
+    </row>
+    <row r="11" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="G11" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="I11" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="K11" s="41">
+        <v>2</v>
+      </c>
+      <c r="L11" s="62" t="s">
+        <v>62</v>
+      </c>
+      <c r="M11" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="N11" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="O11" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="P11" s="37"/>
+    </row>
+    <row r="12" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="60"/>
+      <c r="C12" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="41"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="37"/>
+      <c r="N12" s="37"/>
+      <c r="O12" s="37"/>
+      <c r="P12" s="37"/>
+    </row>
+    <row r="13" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="60"/>
+      <c r="C13" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="G13" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="42"/>
+      <c r="M13" s="37"/>
+      <c r="N13" s="37"/>
+      <c r="O13" s="37"/>
+      <c r="P13" s="37"/>
+    </row>
+    <row r="14" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="60" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="G14" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="H14" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="I14" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="J14" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="K14" s="41">
+        <v>2</v>
+      </c>
+      <c r="L14" s="62" t="s">
+        <v>62</v>
+      </c>
+      <c r="M14" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="N14" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="O14" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="P14" s="37"/>
+    </row>
+    <row r="15" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="60"/>
+      <c r="C15" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="G15" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="41"/>
+      <c r="K15" s="41"/>
+      <c r="L15" s="42"/>
+      <c r="M15" s="37"/>
+      <c r="N15" s="37"/>
+      <c r="O15" s="37"/>
+      <c r="P15" s="37"/>
+    </row>
+    <row r="16" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="60"/>
+      <c r="C16" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="I6" s="61" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6" s="55" t="s">
-        <v>65</v>
-      </c>
-      <c r="K6" s="42">
-        <v>1</v>
-      </c>
-      <c r="L6" s="56" t="s">
-        <v>66</v>
-      </c>
-      <c r="M6" s="44"/>
-      <c r="N6" s="44"/>
-      <c r="O6" s="44"/>
-      <c r="P6" s="44"/>
-    </row>
-    <row r="7" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="54"/>
-      <c r="C7" s="64" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" s="64" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" s="64" t="s">
-        <v>58</v>
-      </c>
-      <c r="F7" s="64" t="s">
-        <v>70</v>
-      </c>
-      <c r="G7" s="64" t="s">
-        <v>4</v>
-      </c>
-      <c r="H7" s="64"/>
-      <c r="I7" s="64"/>
-      <c r="J7" s="42"/>
-      <c r="K7" s="42"/>
-      <c r="L7" s="43"/>
-      <c r="M7" s="44"/>
-      <c r="N7" s="44"/>
-      <c r="O7" s="44"/>
-      <c r="P7" s="44"/>
-    </row>
-    <row r="8" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="54" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="61" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="61" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="61" t="s">
-        <v>55</v>
-      </c>
-      <c r="F8" s="61" t="s">
-        <v>68</v>
-      </c>
-      <c r="G8" s="61" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" s="61" t="s">
-        <v>76</v>
-      </c>
-      <c r="I8" s="61" t="s">
-        <v>23</v>
-      </c>
-      <c r="J8" s="55" t="s">
-        <v>60</v>
-      </c>
-      <c r="K8" s="42">
-        <v>2</v>
-      </c>
-      <c r="L8" s="56" t="s">
-        <v>66</v>
-      </c>
-      <c r="M8" s="53" t="s">
-        <v>56</v>
-      </c>
-      <c r="N8" s="53" t="s">
-        <v>56</v>
-      </c>
-      <c r="O8" s="53" t="s">
-        <v>56</v>
-      </c>
-      <c r="P8" s="44"/>
-    </row>
-    <row r="9" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="54"/>
-      <c r="C9" s="64" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" s="64" t="s">
-        <v>57</v>
-      </c>
-      <c r="E9" s="64" t="s">
-        <v>58</v>
-      </c>
-      <c r="F9" s="64" t="s">
-        <v>71</v>
-      </c>
-      <c r="G9" s="64" t="s">
-        <v>4</v>
-      </c>
-      <c r="H9" s="64"/>
-      <c r="I9" s="64"/>
-      <c r="J9" s="42"/>
-      <c r="K9" s="42"/>
-      <c r="L9" s="43"/>
-      <c r="M9" s="44"/>
-      <c r="N9" s="44"/>
-      <c r="O9" s="44"/>
-      <c r="P9" s="44"/>
-    </row>
-    <row r="10" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="54"/>
-      <c r="C10" s="63" t="s">
-        <v>61</v>
-      </c>
-      <c r="D10" s="63" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" s="63" t="s">
-        <v>59</v>
-      </c>
-      <c r="F10" s="63" t="s">
-        <v>72</v>
-      </c>
-      <c r="G10" s="63" t="s">
-        <v>4</v>
-      </c>
-      <c r="H10" s="63"/>
-      <c r="I10" s="63"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="42"/>
-      <c r="L10" s="43"/>
-      <c r="M10" s="44"/>
-      <c r="N10" s="44"/>
-      <c r="O10" s="44"/>
-      <c r="P10" s="44"/>
-    </row>
-    <row r="11" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="54" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="61" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="61" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="61" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" s="61" t="s">
-        <v>73</v>
-      </c>
-      <c r="G11" s="61" t="s">
-        <v>4</v>
-      </c>
-      <c r="H11" s="61" t="s">
-        <v>76</v>
-      </c>
-      <c r="I11" s="61" t="s">
-        <v>23</v>
-      </c>
-      <c r="J11" s="55" t="s">
-        <v>60</v>
-      </c>
-      <c r="K11" s="42">
-        <v>2</v>
-      </c>
-      <c r="L11" s="56" t="s">
-        <v>66</v>
-      </c>
-      <c r="M11" s="53" t="s">
-        <v>56</v>
-      </c>
-      <c r="N11" s="53" t="s">
-        <v>56</v>
-      </c>
-      <c r="O11" s="53" t="s">
-        <v>56</v>
-      </c>
-      <c r="P11" s="44"/>
-    </row>
-    <row r="12" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="54"/>
-      <c r="C12" s="64" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" s="64" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12" s="64" t="s">
-        <v>58</v>
-      </c>
-      <c r="F12" s="64" t="s">
-        <v>74</v>
-      </c>
-      <c r="G12" s="64" t="s">
-        <v>4</v>
-      </c>
-      <c r="H12" s="64"/>
-      <c r="I12" s="64"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="42"/>
-      <c r="L12" s="43"/>
-      <c r="M12" s="44"/>
-      <c r="N12" s="44"/>
-      <c r="O12" s="44"/>
-      <c r="P12" s="44"/>
-    </row>
-    <row r="13" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="54"/>
-      <c r="C13" s="63" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="63" t="s">
-        <v>62</v>
-      </c>
-      <c r="E13" s="63" t="s">
-        <v>59</v>
-      </c>
-      <c r="F13" s="63" t="s">
-        <v>75</v>
-      </c>
-      <c r="G13" s="63" t="s">
-        <v>4</v>
-      </c>
-      <c r="H13" s="63"/>
-      <c r="I13" s="63"/>
-      <c r="J13" s="42"/>
-      <c r="K13" s="42"/>
-      <c r="L13" s="43"/>
-      <c r="M13" s="44"/>
-      <c r="N13" s="44"/>
-      <c r="O13" s="44"/>
-      <c r="P13" s="44"/>
-    </row>
-    <row r="14" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="54" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="61" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="61" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="61" t="s">
-        <v>55</v>
-      </c>
-      <c r="F14" s="61" t="s">
-        <v>73</v>
-      </c>
-      <c r="G14" s="61" t="s">
-        <v>4</v>
-      </c>
-      <c r="H14" s="61" t="s">
-        <v>76</v>
-      </c>
-      <c r="I14" s="61" t="s">
-        <v>23</v>
-      </c>
-      <c r="J14" s="55" t="s">
-        <v>60</v>
-      </c>
-      <c r="K14" s="42">
-        <v>2</v>
-      </c>
-      <c r="L14" s="56" t="s">
-        <v>66</v>
-      </c>
-      <c r="M14" s="53" t="s">
-        <v>56</v>
-      </c>
-      <c r="N14" s="53" t="s">
-        <v>56</v>
-      </c>
-      <c r="O14" s="53" t="s">
-        <v>56</v>
-      </c>
-      <c r="P14" s="44"/>
-    </row>
-    <row r="15" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="54"/>
-      <c r="C15" s="62" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" s="62" t="s">
-        <v>57</v>
-      </c>
-      <c r="E15" s="62" t="s">
-        <v>58</v>
-      </c>
-      <c r="F15" s="62" t="s">
-        <v>74</v>
-      </c>
-      <c r="G15" s="62" t="s">
-        <v>4</v>
-      </c>
-      <c r="H15" s="62"/>
-      <c r="I15" s="62"/>
-      <c r="J15" s="42"/>
-      <c r="K15" s="42"/>
-      <c r="L15" s="43"/>
-      <c r="M15" s="44"/>
-      <c r="N15" s="44"/>
-      <c r="O15" s="44"/>
-      <c r="P15" s="44"/>
-    </row>
-    <row r="16" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="54"/>
-      <c r="C16" s="63" t="s">
-        <v>61</v>
-      </c>
-      <c r="D16" s="63" t="s">
-        <v>62</v>
-      </c>
-      <c r="E16" s="63" t="s">
-        <v>59</v>
-      </c>
-      <c r="F16" s="63" t="s">
-        <v>75</v>
-      </c>
-      <c r="G16" s="63" t="s">
-        <v>4</v>
-      </c>
-      <c r="H16" s="63"/>
-      <c r="I16" s="63"/>
-      <c r="J16" s="42"/>
-      <c r="K16" s="42"/>
-      <c r="L16" s="43"/>
-      <c r="M16" s="44"/>
-      <c r="N16" s="44"/>
-      <c r="O16" s="44"/>
-      <c r="P16" s="44"/>
+      <c r="G16" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="41"/>
+      <c r="K16" s="41"/>
+      <c r="L16" s="42"/>
+      <c r="M16" s="37"/>
+      <c r="N16" s="37"/>
+      <c r="O16" s="37"/>
+      <c r="P16" s="37"/>
     </row>
     <row r="17" ht="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="B2:P2"/>
-    <mergeCell ref="B3:P3"/>
-    <mergeCell ref="B4:I4"/>
-    <mergeCell ref="J4:P4"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="P6:P7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="J8:J10"/>
-    <mergeCell ref="K8:K10"/>
-    <mergeCell ref="L8:L10"/>
-    <mergeCell ref="M8:M10"/>
-    <mergeCell ref="N8:N10"/>
-    <mergeCell ref="O8:O10"/>
-    <mergeCell ref="P8:P10"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="N6:N7"/>
     <mergeCell ref="O11:O13"/>
     <mergeCell ref="P11:P13"/>
     <mergeCell ref="B14:B16"/>
@@ -2510,6 +2487,26 @@
     <mergeCell ref="L11:L13"/>
     <mergeCell ref="M11:M13"/>
     <mergeCell ref="N11:N13"/>
+    <mergeCell ref="N8:N10"/>
+    <mergeCell ref="O8:O10"/>
+    <mergeCell ref="P8:P10"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="J8:J10"/>
+    <mergeCell ref="K8:K10"/>
+    <mergeCell ref="L8:L10"/>
+    <mergeCell ref="M8:M10"/>
+    <mergeCell ref="B2:P2"/>
+    <mergeCell ref="B3:P3"/>
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="J4:P4"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="P6:P7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="61" fitToHeight="0" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
Cập nhật tài liệu cài đặt nautilous
</commit_message>
<xml_diff>
--- a/tools/IP-Planning-Hardware-Requirements.xlsx
+++ b/tools/IP-Planning-Hardware-Requirements.xlsx
@@ -200,18 +200,12 @@
     <t>+100GB</t>
   </si>
   <si>
-    <t>VLAN82</t>
-  </si>
-  <si>
     <t>+2GB</t>
   </si>
   <si>
     <t>CEPH REPLICATE</t>
   </si>
   <si>
-    <t>VLAN83</t>
-  </si>
-  <si>
     <t>Client1</t>
   </si>
   <si>
@@ -227,43 +221,49 @@
     <t>CEPH Public</t>
   </si>
   <si>
-    <t>VLAN80</t>
-  </si>
-  <si>
-    <t>192.168.80.139</t>
-  </si>
-  <si>
-    <t>192.168.82.139</t>
-  </si>
-  <si>
-    <t>192.168.80.131</t>
-  </si>
-  <si>
-    <t>192.168.80.1</t>
-  </si>
-  <si>
-    <t>192.168.82.131</t>
-  </si>
-  <si>
-    <t>192.168.83.131</t>
-  </si>
-  <si>
-    <t>192.168.80.132</t>
-  </si>
-  <si>
-    <t>192.168.82.132</t>
-  </si>
-  <si>
-    <t>192.168.83.132</t>
-  </si>
-  <si>
-    <t>192.168.82.133</t>
-  </si>
-  <si>
-    <t>192.168.80.133</t>
-  </si>
-  <si>
-    <t>192.168.83.133</t>
+    <t>ens32</t>
+  </si>
+  <si>
+    <t>ens33</t>
+  </si>
+  <si>
+    <t>ens34</t>
+  </si>
+  <si>
+    <t>192.168.98.1</t>
+  </si>
+  <si>
+    <t>192.168.98.85</t>
+  </si>
+  <si>
+    <t>192.168.62.85</t>
+  </si>
+  <si>
+    <t>192.168.63.85</t>
+  </si>
+  <si>
+    <t>192.168.98.86</t>
+  </si>
+  <si>
+    <t>192.168.62.86</t>
+  </si>
+  <si>
+    <t>192.168.63.86</t>
+  </si>
+  <si>
+    <t>192.168.98.87</t>
+  </si>
+  <si>
+    <t>192.168.62.87</t>
+  </si>
+  <si>
+    <t>192.168.63.87</t>
+  </si>
+  <si>
+    <t>192.168.98.80</t>
+  </si>
+  <si>
+    <t>192.168.62.80</t>
   </si>
 </sst>
 </file>
@@ -631,40 +631,49 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -679,13 +688,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -698,18 +710,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1016,23 +1016,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="46" t="s">
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="48"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="42"/>
     </row>
     <row r="3" spans="2:14" ht="33.6" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
@@ -1076,7 +1076,7 @@
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="43" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="30" t="s">
@@ -1094,30 +1094,30 @@
       <c r="G4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="41">
-        <v>4</v>
-      </c>
-      <c r="I4" s="41">
+      <c r="H4" s="45">
+        <v>4</v>
+      </c>
+      <c r="I4" s="45">
         <v>2</v>
       </c>
-      <c r="J4" s="42">
+      <c r="J4" s="46">
         <v>40</v>
       </c>
-      <c r="K4" s="37">
+      <c r="K4" s="47">
         <v>40</v>
       </c>
-      <c r="L4" s="37">
+      <c r="L4" s="47">
         <v>60</v>
       </c>
-      <c r="M4" s="37">
+      <c r="M4" s="47">
         <v>60</v>
       </c>
-      <c r="N4" s="37">
+      <c r="N4" s="47">
         <v>60</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B5" s="39"/>
+      <c r="B5" s="44"/>
       <c r="C5" s="30" t="s">
         <v>2</v>
       </c>
@@ -1129,16 +1129,16 @@
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="42"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
-      <c r="M5" s="37"/>
-      <c r="N5" s="37"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="47"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B6" s="39"/>
+      <c r="B6" s="44"/>
       <c r="C6" s="30" t="s">
         <v>20</v>
       </c>
@@ -1150,16 +1150,16 @@
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="42"/>
-      <c r="K6" s="37"/>
-      <c r="L6" s="37"/>
-      <c r="M6" s="37"/>
-      <c r="N6" s="37"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="47"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="43" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="30" t="s">
@@ -1177,30 +1177,30 @@
       <c r="G7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="41">
-        <v>4</v>
-      </c>
-      <c r="I7" s="41">
+      <c r="H7" s="45">
+        <v>4</v>
+      </c>
+      <c r="I7" s="45">
         <v>2</v>
       </c>
-      <c r="J7" s="42">
+      <c r="J7" s="46">
         <v>40</v>
       </c>
-      <c r="K7" s="37">
+      <c r="K7" s="47">
         <v>40</v>
       </c>
-      <c r="L7" s="37">
+      <c r="L7" s="47">
         <v>60</v>
       </c>
-      <c r="M7" s="37">
+      <c r="M7" s="47">
         <v>60</v>
       </c>
-      <c r="N7" s="37">
+      <c r="N7" s="47">
         <v>60</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="39"/>
+      <c r="B8" s="44"/>
       <c r="C8" s="30" t="s">
         <v>2</v>
       </c>
@@ -1212,16 +1212,16 @@
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="37"/>
-      <c r="M8" s="37"/>
-      <c r="N8" s="37"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="47"/>
+      <c r="N8" s="47"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="40"/>
+      <c r="B9" s="48"/>
       <c r="C9" s="30" t="s">
         <v>20</v>
       </c>
@@ -1233,13 +1233,13 @@
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="42"/>
-      <c r="K9" s="37"/>
-      <c r="L9" s="37"/>
-      <c r="M9" s="37"/>
-      <c r="N9" s="37"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="47"/>
+      <c r="M9" s="47"/>
+      <c r="N9" s="47"/>
     </row>
     <row r="10" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="32" t="s">
@@ -1284,6 +1284,14 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="M7:M9"/>
+    <mergeCell ref="N7:N9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="J7:J9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="L7:L9"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="H2:N2"/>
     <mergeCell ref="B4:B6"/>
@@ -1294,14 +1302,6 @@
     <mergeCell ref="L4:L6"/>
     <mergeCell ref="M4:M6"/>
     <mergeCell ref="N4:N6"/>
-    <mergeCell ref="M7:M9"/>
-    <mergeCell ref="N7:N9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="J7:J9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="L7:L9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="77" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -1334,23 +1334,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="46" t="s">
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="48"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="42"/>
     </row>
     <row r="3" spans="2:14" ht="33.6" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
@@ -1394,7 +1394,7 @@
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="43" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="27" t="s">
@@ -1412,30 +1412,30 @@
       <c r="G4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="41">
-        <v>4</v>
-      </c>
-      <c r="I4" s="41">
+      <c r="H4" s="45">
+        <v>4</v>
+      </c>
+      <c r="I4" s="45">
         <v>2</v>
       </c>
-      <c r="J4" s="42">
+      <c r="J4" s="46">
         <v>40</v>
       </c>
-      <c r="K4" s="37">
+      <c r="K4" s="47">
         <v>40</v>
       </c>
-      <c r="L4" s="37">
+      <c r="L4" s="47">
         <v>60</v>
       </c>
-      <c r="M4" s="37">
+      <c r="M4" s="47">
         <v>60</v>
       </c>
-      <c r="N4" s="37">
+      <c r="N4" s="47">
         <v>60</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B5" s="39"/>
+      <c r="B5" s="44"/>
       <c r="C5" s="27" t="s">
         <v>2</v>
       </c>
@@ -1447,16 +1447,16 @@
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="42"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
-      <c r="M5" s="37"/>
-      <c r="N5" s="37"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="47"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B6" s="39"/>
+      <c r="B6" s="44"/>
       <c r="C6" s="27" t="s">
         <v>20</v>
       </c>
@@ -1468,16 +1468,16 @@
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="42"/>
-      <c r="K6" s="37"/>
-      <c r="L6" s="37"/>
-      <c r="M6" s="37"/>
-      <c r="N6" s="37"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="47"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="43" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="27" t="s">
@@ -1495,30 +1495,30 @@
       <c r="G7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="41">
-        <v>4</v>
-      </c>
-      <c r="I7" s="41">
+      <c r="H7" s="45">
+        <v>4</v>
+      </c>
+      <c r="I7" s="45">
         <v>2</v>
       </c>
-      <c r="J7" s="42">
+      <c r="J7" s="46">
         <v>40</v>
       </c>
-      <c r="K7" s="37">
+      <c r="K7" s="47">
         <v>40</v>
       </c>
-      <c r="L7" s="37">
+      <c r="L7" s="47">
         <v>60</v>
       </c>
-      <c r="M7" s="37">
+      <c r="M7" s="47">
         <v>60</v>
       </c>
-      <c r="N7" s="37">
+      <c r="N7" s="47">
         <v>60</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="39"/>
+      <c r="B8" s="44"/>
       <c r="C8" s="27" t="s">
         <v>2</v>
       </c>
@@ -1530,16 +1530,16 @@
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="37"/>
-      <c r="M8" s="37"/>
-      <c r="N8" s="37"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="47"/>
+      <c r="N8" s="47"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="40"/>
+      <c r="B9" s="48"/>
       <c r="C9" s="27" t="s">
         <v>20</v>
       </c>
@@ -1551,16 +1551,24 @@
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="42"/>
-      <c r="K9" s="37"/>
-      <c r="L9" s="37"/>
-      <c r="M9" s="37"/>
-      <c r="N9" s="37"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="47"/>
+      <c r="M9" s="47"/>
+      <c r="N9" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="M7:M9"/>
+    <mergeCell ref="N7:N9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="J7:J9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="L7:L9"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="H2:N2"/>
     <mergeCell ref="B4:B6"/>
@@ -1571,14 +1579,6 @@
     <mergeCell ref="L4:L6"/>
     <mergeCell ref="M4:M6"/>
     <mergeCell ref="N4:N6"/>
-    <mergeCell ref="M7:M9"/>
-    <mergeCell ref="N7:N9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="J7:J9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="L7:L9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="78" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -1607,40 +1607,40 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="55"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="51"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="46" t="s">
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
-      <c r="N3" s="48"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="42"/>
     </row>
     <row r="4" spans="2:14" ht="33.6" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
@@ -1684,7 +1684,7 @@
       </c>
     </row>
     <row r="5" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="52" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="21" t="s">
@@ -1698,24 +1698,24 @@
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="12"/>
-      <c r="H5" s="51">
+      <c r="H5" s="54">
         <v>6</v>
       </c>
-      <c r="I5" s="41">
+      <c r="I5" s="45">
         <v>2</v>
       </c>
-      <c r="J5" s="42">
+      <c r="J5" s="46">
         <v>100</v>
       </c>
-      <c r="K5" s="37">
+      <c r="K5" s="47">
         <v>60</v>
       </c>
-      <c r="L5" s="37"/>
-      <c r="M5" s="37"/>
-      <c r="N5" s="37"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="47"/>
     </row>
     <row r="6" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="50"/>
+      <c r="B6" s="53"/>
       <c r="C6" s="22" t="s">
         <v>36</v>
       </c>
@@ -1731,16 +1731,16 @@
       <c r="G6" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="51"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="42"/>
-      <c r="K6" s="37"/>
-      <c r="L6" s="37"/>
-      <c r="M6" s="37"/>
-      <c r="N6" s="37"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="47"/>
     </row>
     <row r="7" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="52" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="23" t="s">
@@ -1754,22 +1754,22 @@
       </c>
       <c r="F7" s="15"/>
       <c r="G7" s="16"/>
-      <c r="H7" s="51">
+      <c r="H7" s="54">
         <v>8</v>
       </c>
-      <c r="I7" s="41">
-        <v>4</v>
-      </c>
-      <c r="J7" s="42">
+      <c r="I7" s="45">
+        <v>4</v>
+      </c>
+      <c r="J7" s="46">
         <v>100</v>
       </c>
-      <c r="K7" s="37"/>
-      <c r="L7" s="37"/>
-      <c r="M7" s="37"/>
-      <c r="N7" s="37"/>
+      <c r="K7" s="47"/>
+      <c r="L7" s="47"/>
+      <c r="M7" s="47"/>
+      <c r="N7" s="47"/>
     </row>
     <row r="8" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="50"/>
+      <c r="B8" s="53"/>
       <c r="C8" s="22" t="s">
         <v>36</v>
       </c>
@@ -1785,16 +1785,16 @@
       <c r="G8" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="51"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="37"/>
-      <c r="M8" s="37"/>
-      <c r="N8" s="37"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="47"/>
+      <c r="N8" s="47"/>
     </row>
     <row r="9" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="52" t="s">
         <v>32</v>
       </c>
       <c r="C9" s="23" t="s">
@@ -1808,22 +1808,22 @@
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="16"/>
-      <c r="H9" s="51">
+      <c r="H9" s="54">
         <v>8</v>
       </c>
-      <c r="I9" s="41">
-        <v>4</v>
-      </c>
-      <c r="J9" s="42">
+      <c r="I9" s="45">
+        <v>4</v>
+      </c>
+      <c r="J9" s="46">
         <v>60</v>
       </c>
-      <c r="K9" s="37"/>
-      <c r="L9" s="37"/>
-      <c r="M9" s="37"/>
-      <c r="N9" s="37"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="47"/>
+      <c r="M9" s="47"/>
+      <c r="N9" s="47"/>
     </row>
     <row r="10" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="50"/>
+      <c r="B10" s="53"/>
       <c r="C10" s="22" t="s">
         <v>36</v>
       </c>
@@ -1839,16 +1839,16 @@
       <c r="G10" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="51"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="37"/>
-      <c r="L10" s="37"/>
-      <c r="M10" s="37"/>
-      <c r="N10" s="37"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="47"/>
+      <c r="M10" s="47"/>
+      <c r="N10" s="47"/>
     </row>
     <row r="11" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="49" t="s">
+      <c r="B11" s="52" t="s">
         <v>33</v>
       </c>
       <c r="C11" s="23" t="s">
@@ -1862,30 +1862,30 @@
       </c>
       <c r="F11" s="15"/>
       <c r="G11" s="16"/>
-      <c r="H11" s="51">
+      <c r="H11" s="54">
         <v>8</v>
       </c>
-      <c r="I11" s="41">
-        <v>4</v>
-      </c>
-      <c r="J11" s="42">
+      <c r="I11" s="45">
+        <v>4</v>
+      </c>
+      <c r="J11" s="46">
         <v>60</v>
       </c>
-      <c r="K11" s="37">
+      <c r="K11" s="47">
         <v>50</v>
       </c>
-      <c r="L11" s="37">
+      <c r="L11" s="47">
         <v>50</v>
       </c>
-      <c r="M11" s="37">
+      <c r="M11" s="47">
         <v>50</v>
       </c>
-      <c r="N11" s="37">
+      <c r="N11" s="47">
         <v>50</v>
       </c>
     </row>
     <row r="12" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="50"/>
+      <c r="B12" s="53"/>
       <c r="C12" s="24" t="s">
         <v>36</v>
       </c>
@@ -1901,16 +1901,16 @@
       <c r="G12" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="51"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="37"/>
-      <c r="L12" s="37"/>
-      <c r="M12" s="37"/>
-      <c r="N12" s="37"/>
+      <c r="H12" s="54"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="46"/>
+      <c r="K12" s="47"/>
+      <c r="L12" s="47"/>
+      <c r="M12" s="47"/>
+      <c r="N12" s="47"/>
     </row>
     <row r="13" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="52"/>
+      <c r="B13" s="55"/>
       <c r="C13" s="25" t="s">
         <v>37</v>
       </c>
@@ -1922,37 +1922,16 @@
       </c>
       <c r="F13" s="19"/>
       <c r="G13" s="20"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="41"/>
-      <c r="J13" s="42"/>
-      <c r="K13" s="37"/>
-      <c r="L13" s="37"/>
-      <c r="M13" s="37"/>
-      <c r="N13" s="37"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="45"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="47"/>
+      <c r="M13" s="47"/>
+      <c r="N13" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="H3:N3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
     <mergeCell ref="L11:L13"/>
     <mergeCell ref="M11:M13"/>
     <mergeCell ref="N11:N13"/>
@@ -1967,6 +1946,27 @@
     <mergeCell ref="I11:I13"/>
     <mergeCell ref="J11:J13"/>
     <mergeCell ref="K11:K13"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="H3:N3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -1981,7 +1981,7 @@
   <dimension ref="B2:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
@@ -2002,61 +2002,61 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="22.2" x14ac:dyDescent="0.3">
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="56"/>
-      <c r="N2" s="56"/>
-      <c r="O2" s="56"/>
-      <c r="P2" s="56"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="60"/>
+      <c r="N2" s="60"/>
+      <c r="O2" s="60"/>
+      <c r="P2" s="60"/>
     </row>
     <row r="3" spans="2:16" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="57" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="57"/>
-      <c r="N3" s="57"/>
-      <c r="O3" s="57"/>
-      <c r="P3" s="57"/>
+      <c r="B3" s="61" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="61"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="61"/>
+      <c r="P3" s="61"/>
     </row>
     <row r="4" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="58"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="59" t="s">
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="62"/>
+      <c r="J4" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="59"/>
-      <c r="L4" s="59"/>
-      <c r="M4" s="59"/>
-      <c r="N4" s="59"/>
-      <c r="O4" s="59"/>
-      <c r="P4" s="59"/>
+      <c r="K4" s="63"/>
+      <c r="L4" s="63"/>
+      <c r="M4" s="63"/>
+      <c r="N4" s="63"/>
+      <c r="O4" s="63"/>
+      <c r="P4" s="63"/>
     </row>
     <row r="5" spans="2:16" ht="50.4" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
@@ -2106,371 +2106,391 @@
       </c>
     </row>
     <row r="6" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="60" t="s">
-        <v>59</v>
+      <c r="B6" s="57" t="s">
+        <v>57</v>
       </c>
       <c r="C6" s="34" t="s">
         <v>53</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E6" s="34" t="s">
         <v>1</v>
       </c>
       <c r="F6" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="G6" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="34" t="s">
         <v>65</v>
-      </c>
-      <c r="G6" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="34" t="s">
-        <v>68</v>
       </c>
       <c r="I6" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="J6" s="61" t="s">
+      <c r="J6" s="58" t="s">
+        <v>59</v>
+      </c>
+      <c r="K6" s="45">
+        <v>1</v>
+      </c>
+      <c r="L6" s="59" t="s">
+        <v>60</v>
+      </c>
+      <c r="M6" s="47"/>
+      <c r="N6" s="47"/>
+      <c r="O6" s="47"/>
+      <c r="P6" s="47"/>
+    </row>
+    <row r="7" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="57"/>
+      <c r="C7" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="K6" s="41">
-        <v>1</v>
-      </c>
-      <c r="L6" s="62" t="s">
-        <v>62</v>
-      </c>
-      <c r="M6" s="37"/>
-      <c r="N6" s="37"/>
-      <c r="O6" s="37"/>
-      <c r="P6" s="37"/>
-    </row>
-    <row r="7" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="60"/>
-      <c r="C7" s="36" t="s">
+      <c r="D7" s="36" t="s">
         <v>63</v>
-      </c>
-      <c r="D7" s="36" t="s">
-        <v>55</v>
       </c>
       <c r="E7" s="36" t="s">
         <v>2</v>
       </c>
       <c r="F7" s="36" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="G7" s="36" t="s">
         <v>4</v>
       </c>
       <c r="H7" s="36"/>
       <c r="I7" s="36"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="42"/>
-      <c r="M7" s="37"/>
-      <c r="N7" s="37"/>
-      <c r="O7" s="37"/>
-      <c r="P7" s="37"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="45"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="47"/>
+      <c r="N7" s="47"/>
+      <c r="O7" s="47"/>
+      <c r="P7" s="47"/>
     </row>
     <row r="8" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="60" t="s">
+      <c r="B8" s="57" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="34" t="s">
         <v>53</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E8" s="34" t="s">
         <v>1</v>
       </c>
       <c r="F8" s="34" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G8" s="34" t="s">
         <v>4</v>
       </c>
       <c r="H8" s="34" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I8" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="61" t="s">
-        <v>56</v>
-      </c>
-      <c r="K8" s="41">
+      <c r="J8" s="58" t="s">
+        <v>55</v>
+      </c>
+      <c r="K8" s="45">
         <v>2</v>
       </c>
-      <c r="L8" s="62" t="s">
-        <v>62</v>
-      </c>
-      <c r="M8" s="63" t="s">
+      <c r="L8" s="59" t="s">
+        <v>60</v>
+      </c>
+      <c r="M8" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="N8" s="63" t="s">
+      <c r="N8" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="O8" s="63" t="s">
+      <c r="O8" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="P8" s="37"/>
+      <c r="P8" s="47"/>
     </row>
     <row r="9" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="60"/>
+      <c r="B9" s="57"/>
       <c r="C9" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="36" t="s">
         <v>63</v>
-      </c>
-      <c r="D9" s="36" t="s">
-        <v>55</v>
       </c>
       <c r="E9" s="36" t="s">
         <v>2</v>
       </c>
       <c r="F9" s="36" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G9" s="36" t="s">
         <v>4</v>
       </c>
       <c r="H9" s="36"/>
       <c r="I9" s="36"/>
-      <c r="J9" s="41"/>
-      <c r="K9" s="41"/>
-      <c r="L9" s="42"/>
-      <c r="M9" s="37"/>
-      <c r="N9" s="37"/>
-      <c r="O9" s="37"/>
-      <c r="P9" s="37"/>
+      <c r="J9" s="45"/>
+      <c r="K9" s="45"/>
+      <c r="L9" s="46"/>
+      <c r="M9" s="47"/>
+      <c r="N9" s="47"/>
+      <c r="O9" s="47"/>
+      <c r="P9" s="47"/>
     </row>
     <row r="10" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="60"/>
+      <c r="B10" s="57"/>
       <c r="C10" s="35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="E10" s="35" t="s">
         <v>20</v>
       </c>
       <c r="F10" s="35" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G10" s="35" t="s">
         <v>4</v>
       </c>
       <c r="H10" s="35"/>
       <c r="I10" s="35"/>
-      <c r="J10" s="41"/>
-      <c r="K10" s="41"/>
-      <c r="L10" s="42"/>
-      <c r="M10" s="37"/>
-      <c r="N10" s="37"/>
-      <c r="O10" s="37"/>
-      <c r="P10" s="37"/>
+      <c r="J10" s="45"/>
+      <c r="K10" s="45"/>
+      <c r="L10" s="46"/>
+      <c r="M10" s="47"/>
+      <c r="N10" s="47"/>
+      <c r="O10" s="47"/>
+      <c r="P10" s="47"/>
     </row>
     <row r="11" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="57" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="34" t="s">
         <v>53</v>
       </c>
       <c r="D11" s="34" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E11" s="34" t="s">
         <v>1</v>
       </c>
       <c r="F11" s="34" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G11" s="34" t="s">
         <v>4</v>
       </c>
       <c r="H11" s="34" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I11" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="61" t="s">
-        <v>56</v>
-      </c>
-      <c r="K11" s="41">
+      <c r="J11" s="58" t="s">
+        <v>55</v>
+      </c>
+      <c r="K11" s="45">
         <v>2</v>
       </c>
-      <c r="L11" s="62" t="s">
-        <v>62</v>
-      </c>
-      <c r="M11" s="63" t="s">
+      <c r="L11" s="59" t="s">
+        <v>60</v>
+      </c>
+      <c r="M11" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="N11" s="63" t="s">
+      <c r="N11" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="O11" s="63" t="s">
+      <c r="O11" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="P11" s="37"/>
+      <c r="P11" s="47"/>
     </row>
     <row r="12" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="60"/>
+      <c r="B12" s="57"/>
       <c r="C12" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="36" t="s">
         <v>63</v>
-      </c>
-      <c r="D12" s="36" t="s">
-        <v>55</v>
       </c>
       <c r="E12" s="36" t="s">
         <v>2</v>
       </c>
       <c r="F12" s="36" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G12" s="36" t="s">
         <v>4</v>
       </c>
       <c r="H12" s="36"/>
       <c r="I12" s="36"/>
-      <c r="J12" s="41"/>
-      <c r="K12" s="41"/>
-      <c r="L12" s="42"/>
-      <c r="M12" s="37"/>
-      <c r="N12" s="37"/>
-      <c r="O12" s="37"/>
-      <c r="P12" s="37"/>
+      <c r="J12" s="45"/>
+      <c r="K12" s="45"/>
+      <c r="L12" s="46"/>
+      <c r="M12" s="47"/>
+      <c r="N12" s="47"/>
+      <c r="O12" s="47"/>
+      <c r="P12" s="47"/>
     </row>
     <row r="13" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="60"/>
+      <c r="B13" s="57"/>
       <c r="C13" s="35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D13" s="35" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="E13" s="35" t="s">
         <v>20</v>
       </c>
       <c r="F13" s="35" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G13" s="35" t="s">
         <v>4</v>
       </c>
       <c r="H13" s="35"/>
       <c r="I13" s="35"/>
-      <c r="J13" s="41"/>
-      <c r="K13" s="41"/>
-      <c r="L13" s="42"/>
-      <c r="M13" s="37"/>
-      <c r="N13" s="37"/>
-      <c r="O13" s="37"/>
-      <c r="P13" s="37"/>
+      <c r="J13" s="45"/>
+      <c r="K13" s="45"/>
+      <c r="L13" s="46"/>
+      <c r="M13" s="47"/>
+      <c r="N13" s="47"/>
+      <c r="O13" s="47"/>
+      <c r="P13" s="47"/>
     </row>
     <row r="14" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="60" t="s">
+      <c r="B14" s="57" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="34" t="s">
         <v>53</v>
       </c>
       <c r="D14" s="34" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E14" s="34" t="s">
         <v>1</v>
       </c>
       <c r="F14" s="34" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G14" s="34" t="s">
         <v>4</v>
       </c>
       <c r="H14" s="34" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I14" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="J14" s="61" t="s">
-        <v>56</v>
-      </c>
-      <c r="K14" s="41">
+      <c r="J14" s="58" t="s">
+        <v>55</v>
+      </c>
+      <c r="K14" s="45">
         <v>2</v>
       </c>
-      <c r="L14" s="62" t="s">
-        <v>62</v>
-      </c>
-      <c r="M14" s="63" t="s">
+      <c r="L14" s="59" t="s">
+        <v>60</v>
+      </c>
+      <c r="M14" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="N14" s="63" t="s">
+      <c r="N14" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="O14" s="63" t="s">
+      <c r="O14" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="P14" s="37"/>
+      <c r="P14" s="47"/>
     </row>
     <row r="15" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="60"/>
+      <c r="B15" s="57"/>
       <c r="C15" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="36" t="s">
         <v>63</v>
-      </c>
-      <c r="D15" s="36" t="s">
-        <v>55</v>
       </c>
       <c r="E15" s="36" t="s">
         <v>2</v>
       </c>
       <c r="F15" s="36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G15" s="36" t="s">
         <v>4</v>
       </c>
       <c r="H15" s="36"/>
       <c r="I15" s="36"/>
-      <c r="J15" s="41"/>
-      <c r="K15" s="41"/>
-      <c r="L15" s="42"/>
-      <c r="M15" s="37"/>
-      <c r="N15" s="37"/>
-      <c r="O15" s="37"/>
-      <c r="P15" s="37"/>
+      <c r="J15" s="45"/>
+      <c r="K15" s="45"/>
+      <c r="L15" s="46"/>
+      <c r="M15" s="47"/>
+      <c r="N15" s="47"/>
+      <c r="O15" s="47"/>
+      <c r="P15" s="47"/>
     </row>
     <row r="16" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="60"/>
+      <c r="B16" s="57"/>
       <c r="C16" s="35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D16" s="35" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="E16" s="35" t="s">
         <v>20</v>
       </c>
       <c r="F16" s="35" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G16" s="35" t="s">
         <v>4</v>
       </c>
       <c r="H16" s="35"/>
       <c r="I16" s="35"/>
-      <c r="J16" s="41"/>
-      <c r="K16" s="41"/>
-      <c r="L16" s="42"/>
-      <c r="M16" s="37"/>
-      <c r="N16" s="37"/>
-      <c r="O16" s="37"/>
-      <c r="P16" s="37"/>
+      <c r="J16" s="45"/>
+      <c r="K16" s="45"/>
+      <c r="L16" s="46"/>
+      <c r="M16" s="47"/>
+      <c r="N16" s="47"/>
+      <c r="O16" s="47"/>
+      <c r="P16" s="47"/>
     </row>
     <row r="17" ht="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="B2:P2"/>
+    <mergeCell ref="B3:P3"/>
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="J4:P4"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="P6:P7"/>
+    <mergeCell ref="N8:N10"/>
+    <mergeCell ref="O8:O10"/>
+    <mergeCell ref="P8:P10"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="J8:J10"/>
+    <mergeCell ref="K8:K10"/>
+    <mergeCell ref="L8:L10"/>
+    <mergeCell ref="M8:M10"/>
     <mergeCell ref="O11:O13"/>
     <mergeCell ref="P11:P13"/>
     <mergeCell ref="B14:B16"/>
@@ -2487,26 +2507,6 @@
     <mergeCell ref="L11:L13"/>
     <mergeCell ref="M11:M13"/>
     <mergeCell ref="N11:N13"/>
-    <mergeCell ref="N8:N10"/>
-    <mergeCell ref="O8:O10"/>
-    <mergeCell ref="P8:P10"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="J8:J10"/>
-    <mergeCell ref="K8:K10"/>
-    <mergeCell ref="L8:L10"/>
-    <mergeCell ref="M8:M10"/>
-    <mergeCell ref="B2:P2"/>
-    <mergeCell ref="B3:P3"/>
-    <mergeCell ref="B4:I4"/>
-    <mergeCell ref="J4:P4"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="P6:P7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="61" fitToHeight="0" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
Cap nhat huong dan
</commit_message>
<xml_diff>
--- a/tools/IP-Planning-Hardware-Requirements.xlsx
+++ b/tools/IP-Planning-Hardware-Requirements.xlsx
@@ -260,10 +260,10 @@
     <t>192.168.63.87</t>
   </si>
   <si>
-    <t>192.168.98.80</t>
-  </si>
-  <si>
-    <t>192.168.62.80</t>
+    <t>192.168.98.84</t>
+  </si>
+  <si>
+    <t>192.168.62.84</t>
   </si>
 </sst>
 </file>
@@ -631,6 +631,24 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -649,22 +667,16 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -676,16 +688,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -698,18 +710,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1016,23 +1016,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="40" t="s">
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="42"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="48"/>
     </row>
     <row r="3" spans="2:14" ht="33.6" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
@@ -1076,7 +1076,7 @@
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="38" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="30" t="s">
@@ -1094,30 +1094,30 @@
       <c r="G4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="45">
-        <v>4</v>
-      </c>
-      <c r="I4" s="45">
+      <c r="H4" s="41">
+        <v>4</v>
+      </c>
+      <c r="I4" s="41">
         <v>2</v>
       </c>
-      <c r="J4" s="46">
+      <c r="J4" s="42">
         <v>40</v>
       </c>
-      <c r="K4" s="47">
+      <c r="K4" s="37">
         <v>40</v>
       </c>
-      <c r="L4" s="47">
+      <c r="L4" s="37">
         <v>60</v>
       </c>
-      <c r="M4" s="47">
+      <c r="M4" s="37">
         <v>60</v>
       </c>
-      <c r="N4" s="47">
+      <c r="N4" s="37">
         <v>60</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B5" s="44"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="30" t="s">
         <v>2</v>
       </c>
@@ -1129,16 +1129,16 @@
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="47"/>
-      <c r="L5" s="47"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="47"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="37"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B6" s="44"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="30" t="s">
         <v>20</v>
       </c>
@@ -1150,16 +1150,16 @@
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="47"/>
-      <c r="N6" s="47"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="38" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="30" t="s">
@@ -1177,30 +1177,30 @@
       <c r="G7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="45">
-        <v>4</v>
-      </c>
-      <c r="I7" s="45">
+      <c r="H7" s="41">
+        <v>4</v>
+      </c>
+      <c r="I7" s="41">
         <v>2</v>
       </c>
-      <c r="J7" s="46">
+      <c r="J7" s="42">
         <v>40</v>
       </c>
-      <c r="K7" s="47">
+      <c r="K7" s="37">
         <v>40</v>
       </c>
-      <c r="L7" s="47">
+      <c r="L7" s="37">
         <v>60</v>
       </c>
-      <c r="M7" s="47">
+      <c r="M7" s="37">
         <v>60</v>
       </c>
-      <c r="N7" s="47">
+      <c r="N7" s="37">
         <v>60</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="44"/>
+      <c r="B8" s="39"/>
       <c r="C8" s="30" t="s">
         <v>2</v>
       </c>
@@ -1212,16 +1212,16 @@
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="46"/>
-      <c r="K8" s="47"/>
-      <c r="L8" s="47"/>
-      <c r="M8" s="47"/>
-      <c r="N8" s="47"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="37"/>
+      <c r="N8" s="37"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="48"/>
+      <c r="B9" s="40"/>
       <c r="C9" s="30" t="s">
         <v>20</v>
       </c>
@@ -1233,13 +1233,13 @@
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="46"/>
-      <c r="K9" s="47"/>
-      <c r="L9" s="47"/>
-      <c r="M9" s="47"/>
-      <c r="N9" s="47"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
     </row>
     <row r="10" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="32" t="s">
@@ -1284,14 +1284,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="M7:M9"/>
-    <mergeCell ref="N7:N9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="J7:J9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="L7:L9"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="H2:N2"/>
     <mergeCell ref="B4:B6"/>
@@ -1302,6 +1294,14 @@
     <mergeCell ref="L4:L6"/>
     <mergeCell ref="M4:M6"/>
     <mergeCell ref="N4:N6"/>
+    <mergeCell ref="M7:M9"/>
+    <mergeCell ref="N7:N9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="J7:J9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="L7:L9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="77" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -1334,23 +1334,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="40" t="s">
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="42"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="48"/>
     </row>
     <row r="3" spans="2:14" ht="33.6" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
@@ -1394,7 +1394,7 @@
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="38" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="27" t="s">
@@ -1412,30 +1412,30 @@
       <c r="G4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="45">
-        <v>4</v>
-      </c>
-      <c r="I4" s="45">
+      <c r="H4" s="41">
+        <v>4</v>
+      </c>
+      <c r="I4" s="41">
         <v>2</v>
       </c>
-      <c r="J4" s="46">
+      <c r="J4" s="42">
         <v>40</v>
       </c>
-      <c r="K4" s="47">
+      <c r="K4" s="37">
         <v>40</v>
       </c>
-      <c r="L4" s="47">
+      <c r="L4" s="37">
         <v>60</v>
       </c>
-      <c r="M4" s="47">
+      <c r="M4" s="37">
         <v>60</v>
       </c>
-      <c r="N4" s="47">
+      <c r="N4" s="37">
         <v>60</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B5" s="44"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="27" t="s">
         <v>2</v>
       </c>
@@ -1447,16 +1447,16 @@
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="47"/>
-      <c r="L5" s="47"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="47"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="37"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B6" s="44"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="27" t="s">
         <v>20</v>
       </c>
@@ -1468,16 +1468,16 @@
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="47"/>
-      <c r="N6" s="47"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="38" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="27" t="s">
@@ -1495,30 +1495,30 @@
       <c r="G7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="45">
-        <v>4</v>
-      </c>
-      <c r="I7" s="45">
+      <c r="H7" s="41">
+        <v>4</v>
+      </c>
+      <c r="I7" s="41">
         <v>2</v>
       </c>
-      <c r="J7" s="46">
+      <c r="J7" s="42">
         <v>40</v>
       </c>
-      <c r="K7" s="47">
+      <c r="K7" s="37">
         <v>40</v>
       </c>
-      <c r="L7" s="47">
+      <c r="L7" s="37">
         <v>60</v>
       </c>
-      <c r="M7" s="47">
+      <c r="M7" s="37">
         <v>60</v>
       </c>
-      <c r="N7" s="47">
+      <c r="N7" s="37">
         <v>60</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="44"/>
+      <c r="B8" s="39"/>
       <c r="C8" s="27" t="s">
         <v>2</v>
       </c>
@@ -1530,16 +1530,16 @@
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="46"/>
-      <c r="K8" s="47"/>
-      <c r="L8" s="47"/>
-      <c r="M8" s="47"/>
-      <c r="N8" s="47"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="37"/>
+      <c r="N8" s="37"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="48"/>
+      <c r="B9" s="40"/>
       <c r="C9" s="27" t="s">
         <v>20</v>
       </c>
@@ -1551,24 +1551,16 @@
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="46"/>
-      <c r="K9" s="47"/>
-      <c r="L9" s="47"/>
-      <c r="M9" s="47"/>
-      <c r="N9" s="47"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="M7:M9"/>
-    <mergeCell ref="N7:N9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="J7:J9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="L7:L9"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="H2:N2"/>
     <mergeCell ref="B4:B6"/>
@@ -1579,6 +1571,14 @@
     <mergeCell ref="L4:L6"/>
     <mergeCell ref="M4:M6"/>
     <mergeCell ref="N4:N6"/>
+    <mergeCell ref="M7:M9"/>
+    <mergeCell ref="N7:N9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="J7:J9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="L7:L9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="78" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -1607,40 +1607,40 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="50"/>
-      <c r="N2" s="51"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="55"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="40" t="s">
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="42"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="48"/>
     </row>
     <row r="4" spans="2:14" ht="33.6" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
@@ -1684,7 +1684,7 @@
       </c>
     </row>
     <row r="5" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="49" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="21" t="s">
@@ -1698,24 +1698,24 @@
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="12"/>
-      <c r="H5" s="54">
+      <c r="H5" s="51">
         <v>6</v>
       </c>
-      <c r="I5" s="45">
+      <c r="I5" s="41">
         <v>2</v>
       </c>
-      <c r="J5" s="46">
+      <c r="J5" s="42">
         <v>100</v>
       </c>
-      <c r="K5" s="47">
+      <c r="K5" s="37">
         <v>60</v>
       </c>
-      <c r="L5" s="47"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="47"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="37"/>
     </row>
     <row r="6" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="53"/>
+      <c r="B6" s="50"/>
       <c r="C6" s="22" t="s">
         <v>36</v>
       </c>
@@ -1731,16 +1731,16 @@
       <c r="G6" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="54"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="47"/>
-      <c r="N6" s="47"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
     </row>
     <row r="7" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="52" t="s">
+      <c r="B7" s="49" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="23" t="s">
@@ -1754,22 +1754,22 @@
       </c>
       <c r="F7" s="15"/>
       <c r="G7" s="16"/>
-      <c r="H7" s="54">
+      <c r="H7" s="51">
         <v>8</v>
       </c>
-      <c r="I7" s="45">
-        <v>4</v>
-      </c>
-      <c r="J7" s="46">
+      <c r="I7" s="41">
+        <v>4</v>
+      </c>
+      <c r="J7" s="42">
         <v>100</v>
       </c>
-      <c r="K7" s="47"/>
-      <c r="L7" s="47"/>
-      <c r="M7" s="47"/>
-      <c r="N7" s="47"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="37"/>
     </row>
     <row r="8" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="53"/>
+      <c r="B8" s="50"/>
       <c r="C8" s="22" t="s">
         <v>36</v>
       </c>
@@ -1785,16 +1785,16 @@
       <c r="G8" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="54"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="46"/>
-      <c r="K8" s="47"/>
-      <c r="L8" s="47"/>
-      <c r="M8" s="47"/>
-      <c r="N8" s="47"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="37"/>
+      <c r="N8" s="37"/>
     </row>
     <row r="9" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="49" t="s">
         <v>32</v>
       </c>
       <c r="C9" s="23" t="s">
@@ -1808,22 +1808,22 @@
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="16"/>
-      <c r="H9" s="54">
+      <c r="H9" s="51">
         <v>8</v>
       </c>
-      <c r="I9" s="45">
-        <v>4</v>
-      </c>
-      <c r="J9" s="46">
+      <c r="I9" s="41">
+        <v>4</v>
+      </c>
+      <c r="J9" s="42">
         <v>60</v>
       </c>
-      <c r="K9" s="47"/>
-      <c r="L9" s="47"/>
-      <c r="M9" s="47"/>
-      <c r="N9" s="47"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
     </row>
     <row r="10" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="53"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="22" t="s">
         <v>36</v>
       </c>
@@ -1839,16 +1839,16 @@
       <c r="G10" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="54"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="46"/>
-      <c r="K10" s="47"/>
-      <c r="L10" s="47"/>
-      <c r="M10" s="47"/>
-      <c r="N10" s="47"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="37"/>
+      <c r="M10" s="37"/>
+      <c r="N10" s="37"/>
     </row>
     <row r="11" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="52" t="s">
+      <c r="B11" s="49" t="s">
         <v>33</v>
       </c>
       <c r="C11" s="23" t="s">
@@ -1862,30 +1862,30 @@
       </c>
       <c r="F11" s="15"/>
       <c r="G11" s="16"/>
-      <c r="H11" s="54">
+      <c r="H11" s="51">
         <v>8</v>
       </c>
-      <c r="I11" s="45">
-        <v>4</v>
-      </c>
-      <c r="J11" s="46">
+      <c r="I11" s="41">
+        <v>4</v>
+      </c>
+      <c r="J11" s="42">
         <v>60</v>
       </c>
-      <c r="K11" s="47">
+      <c r="K11" s="37">
         <v>50</v>
       </c>
-      <c r="L11" s="47">
+      <c r="L11" s="37">
         <v>50</v>
       </c>
-      <c r="M11" s="47">
+      <c r="M11" s="37">
         <v>50</v>
       </c>
-      <c r="N11" s="47">
+      <c r="N11" s="37">
         <v>50</v>
       </c>
     </row>
     <row r="12" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="53"/>
+      <c r="B12" s="50"/>
       <c r="C12" s="24" t="s">
         <v>36</v>
       </c>
@@ -1901,16 +1901,16 @@
       <c r="G12" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="54"/>
-      <c r="I12" s="45"/>
-      <c r="J12" s="46"/>
-      <c r="K12" s="47"/>
-      <c r="L12" s="47"/>
-      <c r="M12" s="47"/>
-      <c r="N12" s="47"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="37"/>
+      <c r="N12" s="37"/>
     </row>
     <row r="13" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="55"/>
+      <c r="B13" s="52"/>
       <c r="C13" s="25" t="s">
         <v>37</v>
       </c>
@@ -1922,16 +1922,37 @@
       </c>
       <c r="F13" s="19"/>
       <c r="G13" s="20"/>
-      <c r="H13" s="54"/>
-      <c r="I13" s="45"/>
-      <c r="J13" s="46"/>
-      <c r="K13" s="47"/>
-      <c r="L13" s="47"/>
-      <c r="M13" s="47"/>
-      <c r="N13" s="47"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="42"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="37"/>
+      <c r="M13" s="37"/>
+      <c r="N13" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="H3:N3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
     <mergeCell ref="L11:L13"/>
     <mergeCell ref="M11:M13"/>
     <mergeCell ref="N11:N13"/>
@@ -1946,27 +1967,6 @@
     <mergeCell ref="I11:I13"/>
     <mergeCell ref="J11:J13"/>
     <mergeCell ref="K11:K13"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="H3:N3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -1981,7 +1981,7 @@
   <dimension ref="B2:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
@@ -2002,61 +2002,61 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="22.2" x14ac:dyDescent="0.3">
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="60"/>
-      <c r="O2" s="60"/>
-      <c r="P2" s="60"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="56"/>
+      <c r="P2" s="56"/>
     </row>
     <row r="3" spans="2:16" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="61" t="s">
+      <c r="B3" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="61"/>
-      <c r="K3" s="61"/>
-      <c r="L3" s="61"/>
-      <c r="M3" s="61"/>
-      <c r="N3" s="61"/>
-      <c r="O3" s="61"/>
-      <c r="P3" s="61"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="57"/>
+      <c r="P3" s="57"/>
     </row>
     <row r="4" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="62"/>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
-      <c r="I4" s="62"/>
-      <c r="J4" s="63" t="s">
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="58"/>
+      <c r="J4" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="63"/>
-      <c r="L4" s="63"/>
-      <c r="M4" s="63"/>
-      <c r="N4" s="63"/>
-      <c r="O4" s="63"/>
-      <c r="P4" s="63"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="59"/>
+      <c r="N4" s="59"/>
+      <c r="O4" s="59"/>
+      <c r="P4" s="59"/>
     </row>
     <row r="5" spans="2:16" ht="50.4" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
@@ -2106,7 +2106,7 @@
       </c>
     </row>
     <row r="6" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="61" t="s">
         <v>57</v>
       </c>
       <c r="C6" s="34" t="s">
@@ -2130,22 +2130,22 @@
       <c r="I6" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="J6" s="58" t="s">
+      <c r="J6" s="62" t="s">
         <v>59</v>
       </c>
-      <c r="K6" s="45">
+      <c r="K6" s="41">
         <v>1</v>
       </c>
-      <c r="L6" s="59" t="s">
+      <c r="L6" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="M6" s="47"/>
-      <c r="N6" s="47"/>
-      <c r="O6" s="47"/>
-      <c r="P6" s="47"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
+      <c r="O6" s="37"/>
+      <c r="P6" s="37"/>
     </row>
     <row r="7" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="57"/>
+      <c r="B7" s="61"/>
       <c r="C7" s="36" t="s">
         <v>61</v>
       </c>
@@ -2163,16 +2163,16 @@
       </c>
       <c r="H7" s="36"/>
       <c r="I7" s="36"/>
-      <c r="J7" s="45"/>
-      <c r="K7" s="45"/>
-      <c r="L7" s="46"/>
-      <c r="M7" s="47"/>
-      <c r="N7" s="47"/>
-      <c r="O7" s="47"/>
-      <c r="P7" s="47"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="37"/>
+      <c r="O7" s="37"/>
+      <c r="P7" s="37"/>
     </row>
     <row r="8" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="61" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="34" t="s">
@@ -2196,28 +2196,28 @@
       <c r="I8" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="58" t="s">
+      <c r="J8" s="62" t="s">
         <v>55</v>
       </c>
-      <c r="K8" s="45">
+      <c r="K8" s="41">
         <v>2</v>
       </c>
-      <c r="L8" s="59" t="s">
+      <c r="L8" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="M8" s="56" t="s">
+      <c r="M8" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="N8" s="56" t="s">
+      <c r="N8" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="O8" s="56" t="s">
+      <c r="O8" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="P8" s="47"/>
+      <c r="P8" s="37"/>
     </row>
     <row r="9" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="57"/>
+      <c r="B9" s="61"/>
       <c r="C9" s="36" t="s">
         <v>61</v>
       </c>
@@ -2235,16 +2235,16 @@
       </c>
       <c r="H9" s="36"/>
       <c r="I9" s="36"/>
-      <c r="J9" s="45"/>
-      <c r="K9" s="45"/>
-      <c r="L9" s="46"/>
-      <c r="M9" s="47"/>
-      <c r="N9" s="47"/>
-      <c r="O9" s="47"/>
-      <c r="P9" s="47"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
+      <c r="O9" s="37"/>
+      <c r="P9" s="37"/>
     </row>
     <row r="10" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="57"/>
+      <c r="B10" s="61"/>
       <c r="C10" s="35" t="s">
         <v>56</v>
       </c>
@@ -2262,16 +2262,16 @@
       </c>
       <c r="H10" s="35"/>
       <c r="I10" s="35"/>
-      <c r="J10" s="45"/>
-      <c r="K10" s="45"/>
-      <c r="L10" s="46"/>
-      <c r="M10" s="47"/>
-      <c r="N10" s="47"/>
-      <c r="O10" s="47"/>
-      <c r="P10" s="47"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="37"/>
+      <c r="N10" s="37"/>
+      <c r="O10" s="37"/>
+      <c r="P10" s="37"/>
     </row>
     <row r="11" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="57" t="s">
+      <c r="B11" s="61" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="34" t="s">
@@ -2295,28 +2295,28 @@
       <c r="I11" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="58" t="s">
+      <c r="J11" s="62" t="s">
         <v>55</v>
       </c>
-      <c r="K11" s="45">
+      <c r="K11" s="41">
         <v>2</v>
       </c>
-      <c r="L11" s="59" t="s">
+      <c r="L11" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="M11" s="56" t="s">
+      <c r="M11" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="N11" s="56" t="s">
+      <c r="N11" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="O11" s="56" t="s">
+      <c r="O11" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="P11" s="47"/>
+      <c r="P11" s="37"/>
     </row>
     <row r="12" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="57"/>
+      <c r="B12" s="61"/>
       <c r="C12" s="36" t="s">
         <v>61</v>
       </c>
@@ -2334,16 +2334,16 @@
       </c>
       <c r="H12" s="36"/>
       <c r="I12" s="36"/>
-      <c r="J12" s="45"/>
-      <c r="K12" s="45"/>
-      <c r="L12" s="46"/>
-      <c r="M12" s="47"/>
-      <c r="N12" s="47"/>
-      <c r="O12" s="47"/>
-      <c r="P12" s="47"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="41"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="37"/>
+      <c r="N12" s="37"/>
+      <c r="O12" s="37"/>
+      <c r="P12" s="37"/>
     </row>
     <row r="13" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="57"/>
+      <c r="B13" s="61"/>
       <c r="C13" s="35" t="s">
         <v>56</v>
       </c>
@@ -2361,16 +2361,16 @@
       </c>
       <c r="H13" s="35"/>
       <c r="I13" s="35"/>
-      <c r="J13" s="45"/>
-      <c r="K13" s="45"/>
-      <c r="L13" s="46"/>
-      <c r="M13" s="47"/>
-      <c r="N13" s="47"/>
-      <c r="O13" s="47"/>
-      <c r="P13" s="47"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="42"/>
+      <c r="M13" s="37"/>
+      <c r="N13" s="37"/>
+      <c r="O13" s="37"/>
+      <c r="P13" s="37"/>
     </row>
     <row r="14" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="57" t="s">
+      <c r="B14" s="61" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="34" t="s">
@@ -2394,28 +2394,28 @@
       <c r="I14" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="J14" s="58" t="s">
+      <c r="J14" s="62" t="s">
         <v>55</v>
       </c>
-      <c r="K14" s="45">
+      <c r="K14" s="41">
         <v>2</v>
       </c>
-      <c r="L14" s="59" t="s">
+      <c r="L14" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="M14" s="56" t="s">
+      <c r="M14" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="N14" s="56" t="s">
+      <c r="N14" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="O14" s="56" t="s">
+      <c r="O14" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="P14" s="47"/>
+      <c r="P14" s="37"/>
     </row>
     <row r="15" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="57"/>
+      <c r="B15" s="61"/>
       <c r="C15" s="36" t="s">
         <v>61</v>
       </c>
@@ -2433,16 +2433,16 @@
       </c>
       <c r="H15" s="36"/>
       <c r="I15" s="36"/>
-      <c r="J15" s="45"/>
-      <c r="K15" s="45"/>
-      <c r="L15" s="46"/>
-      <c r="M15" s="47"/>
-      <c r="N15" s="47"/>
-      <c r="O15" s="47"/>
-      <c r="P15" s="47"/>
+      <c r="J15" s="41"/>
+      <c r="K15" s="41"/>
+      <c r="L15" s="42"/>
+      <c r="M15" s="37"/>
+      <c r="N15" s="37"/>
+      <c r="O15" s="37"/>
+      <c r="P15" s="37"/>
     </row>
     <row r="16" spans="2:16" s="33" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="57"/>
+      <c r="B16" s="61"/>
       <c r="C16" s="35" t="s">
         <v>56</v>
       </c>
@@ -2460,37 +2460,17 @@
       </c>
       <c r="H16" s="35"/>
       <c r="I16" s="35"/>
-      <c r="J16" s="45"/>
-      <c r="K16" s="45"/>
-      <c r="L16" s="46"/>
-      <c r="M16" s="47"/>
-      <c r="N16" s="47"/>
-      <c r="O16" s="47"/>
-      <c r="P16" s="47"/>
+      <c r="J16" s="41"/>
+      <c r="K16" s="41"/>
+      <c r="L16" s="42"/>
+      <c r="M16" s="37"/>
+      <c r="N16" s="37"/>
+      <c r="O16" s="37"/>
+      <c r="P16" s="37"/>
     </row>
     <row r="17" ht="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="B2:P2"/>
-    <mergeCell ref="B3:P3"/>
-    <mergeCell ref="B4:I4"/>
-    <mergeCell ref="J4:P4"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="P6:P7"/>
-    <mergeCell ref="N8:N10"/>
-    <mergeCell ref="O8:O10"/>
-    <mergeCell ref="P8:P10"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="J8:J10"/>
-    <mergeCell ref="K8:K10"/>
-    <mergeCell ref="L8:L10"/>
-    <mergeCell ref="M8:M10"/>
     <mergeCell ref="O11:O13"/>
     <mergeCell ref="P11:P13"/>
     <mergeCell ref="B14:B16"/>
@@ -2507,6 +2487,26 @@
     <mergeCell ref="L11:L13"/>
     <mergeCell ref="M11:M13"/>
     <mergeCell ref="N11:N13"/>
+    <mergeCell ref="N8:N10"/>
+    <mergeCell ref="O8:O10"/>
+    <mergeCell ref="P8:P10"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="J8:J10"/>
+    <mergeCell ref="K8:K10"/>
+    <mergeCell ref="L8:L10"/>
+    <mergeCell ref="M8:M10"/>
+    <mergeCell ref="B2:P2"/>
+    <mergeCell ref="B3:P3"/>
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="J4:P4"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="P6:P7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="61" fitToHeight="0" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>